<commit_message>
Changed calculation steps name
</commit_message>
<xml_diff>
--- a/docs/Calculation algorithm.xlsx
+++ b/docs/Calculation algorithm.xlsx
@@ -4,16 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inverse kinematic" sheetId="1" r:id="rId1"/>
     <sheet name="Advance trajectory" sheetId="6" r:id="rId2"/>
     <sheet name="Joystick smooth" sheetId="7" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="144525" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -137,15 +134,9 @@
     <t xml:space="preserve">z0 = </t>
   </si>
   <si>
-    <t xml:space="preserve">Макс. длина шага = </t>
-  </si>
-  <si>
     <t xml:space="preserve">Кривизна [-1.99; 1.99] = </t>
   </si>
   <si>
-    <t xml:space="preserve">Длина шага [мм] = </t>
-  </si>
-  <si>
     <t>Общие вычисления</t>
   </si>
   <si>
@@ -171,12 +162,6 @@
   </si>
   <si>
     <t>Магия из неизвестной области математики, но она работает</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Радиус кривизны через кривизну = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Макс. угол дуги траектории = </t>
   </si>
   <si>
     <t>Вычисляется через формулу длины дуги (длина = угол в радианах * радиус)</t>
@@ -254,6 +239,18 @@
   </si>
   <si>
     <t xml:space="preserve">k = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Расстояние [мм] = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Радиус траектории тела = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Макс. Радиус траектории = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Макс. угол дуги = </t>
   </si>
 </sst>
 </file>
@@ -1226,6 +1223,132 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1271,18 +1394,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1290,120 +1401,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1531,67 +1528,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-13.552609231287864</c:v>
+                  <c:v>-14.668890498750928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-14.256273394168016</c:v>
+                  <c:v>-15.262125378436776</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-14.94830033682395</c:v>
+                  <c:v>-15.842792873173584</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-15.628125228428157</c:v>
+                  <c:v>-16.410583064121127</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-16.295193197439634</c:v>
+                  <c:v>-16.965192905424296</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-16.94895978448875</c:v>
+                  <c:v>-17.506326385957379</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-17.58889138676383</c:v>
+                  <c:v>-18.033694687313591</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-18.2144656935365</c:v>
+                  <c:v>-18.547016337955782</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-18.825172112470568</c:v>
+                  <c:v>-19.046017363445763</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.420512186366274</c:v>
+                  <c:v>-19.53043143267238</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-20.563162576727148</c:v>
+                  <c:v>-20.454472443261693</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-21.109540264524604</c:v>
+                  <c:v>-20.893606197523482</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-21.63868711115769</c:v>
+                  <c:v>-21.317166884548143</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-22.150171228165355</c:v>
+                  <c:v>-21.724928437889609</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-22.643575143366586</c:v>
+                  <c:v>-22.116673223551054</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-23.118496141600247</c:v>
+                  <c:v>-22.492192156142416</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-23.574546593420266</c:v>
+                  <c:v>-22.851284810475221</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-24.011354271477963</c:v>
+                  <c:v>-23.19375952853526</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-24.42856265433311</c:v>
+                  <c:v>-23.519433521775909</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-24.825831217445973</c:v>
+                  <c:v>-23.82813296867765</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1603,67 +1600,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>24.826337589332955</c:v>
+                  <c:v>25.945180011944267</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.429013761510788</c:v>
+                  <c:v>25.408014600434004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.011751027834091</c:v>
+                  <c:v>24.857288205247652</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.574889957203627</c:v>
+                  <c:v>24.293294764804742</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.118787114638497</c:v>
+                  <c:v>23.716335298526101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.643814770248621</c:v>
+                  <c:v>23.126717746171163</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.150360595388669</c:v>
+                  <c:v>22.524756803481743</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.638827346241598</c:v>
+                  <c:v>21.910773754219893</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.109632535089961</c:v>
+                  <c:v>21.285096298689638</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.563208089543348</c:v>
+                  <c:v>20.648058378833856</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20</c:v>
+                  <c:v>20.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.420467955630489</c:v>
+                  <c:v>19.341267049469508</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.825084969180441</c:v>
+                  <c:v>18.67221111184783</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.214336990898609</c:v>
+                  <c:v>17.993189281413734</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.588722511905392</c:v>
+                  <c:v>17.304563971527834</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.948752157325458</c:v>
+                  <c:v>16.606702721202282</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.294948269516713</c:v>
+                  <c:v>15.899977998934611</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.627844481735664</c:v>
+                  <c:v>15.184767003910704</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.94798528258711</c:v>
+                  <c:v>14.461451464682787</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.255925571613801</c:v>
+                  <c:v>13.730417435430004</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.552230206388673</c:v>
+                  <c:v>12.992055089910252</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1683,67 +1680,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-33.58118314776253</c:v>
+                  <c:v>-33.849974896909728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-33.849270274172284</c:v>
+                  <c:v>-34.067691463555342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-34.089728420558906</c:v>
+                  <c:v>-34.26280357707833</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-34.302361325526448</c:v>
+                  <c:v>-34.435207100566458</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-34.486995438578141</c:v>
+                  <c:v>-34.584810017331115</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-34.643480061767946</c:v>
+                  <c:v>-34.711532480019251</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-34.771687472699867</c:v>
+                  <c:v>-34.815306853230183</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-34.871513028774679</c:v>
+                  <c:v>-34.896077749614562</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-34.942875252598988</c:v>
+                  <c:v>-34.953802059436164</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-34.985715898486902</c:v>
+                  <c:v>-34.988448973580795</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>-35</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-34.985715898486902</c:v>
+                  <c:v>-34.988448973580795</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-34.942875252598988</c:v>
+                  <c:v>-34.953802059436164</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-34.871513028774679</c:v>
+                  <c:v>-34.896077749614562</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-34.771687472699867</c:v>
+                  <c:v>-34.81530685323019</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-34.643480061767946</c:v>
+                  <c:v>-34.711532480019251</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-34.486995438578141</c:v>
+                  <c:v>-34.584810017331122</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-34.302361325526448</c:v>
+                  <c:v>-34.435207100566458</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-34.089728420558906</c:v>
+                  <c:v>-34.26280357707833</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-33.849270274172284</c:v>
+                  <c:v>-34.067691463555342</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-33.581183147762538</c:v>
+                  <c:v>-33.849974896909735</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1755,67 +1752,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>9.8645119362814189</c:v>
+                  <c:v>9.9112783872395323</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.9011525675104046</c:v>
+                  <c:v>8.9352891362541804</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.9305280981187476</c:v>
+                  <c:v>7.9545308660430658</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9534307496060261</c:v>
+                  <c:v>6.9695270353298122</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9706580266211331</c:v>
+                  <c:v>5.9808033688150415</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9830120660407724</c:v>
+                  <c:v>4.9888875765820719</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.9912989822672147</c:v>
+                  <c:v>3.9943090724429657</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.9963282092794445</c:v>
+                  <c:v>2.9975986913752215</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.998911839975027</c:v>
+                  <c:v>1.9992884062000542</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99986396334176308</c:v>
+                  <c:v>0.99991104365317329</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.2882120380498403E-15</c:v>
+                  <c:v>5.3029658040673552E-15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-0.99986396334175442</c:v>
+                  <c:v>-0.99991104365316275</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.9989118399750183</c:v>
+                  <c:v>-1.9992884062000433</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2.9963282092794357</c:v>
+                  <c:v>-2.9975986913752113</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-3.9912989822672063</c:v>
+                  <c:v>-3.994309072442936</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-4.9830120660407644</c:v>
+                  <c:v>-4.9888875765820613</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-5.9706580266211242</c:v>
+                  <c:v>-5.9808033688150299</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-6.9534307496060181</c:v>
+                  <c:v>-6.9695270353298016</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-7.9305280981187396</c:v>
+                  <c:v>-7.9545308660430551</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-8.9011525675103975</c:v>
+                  <c:v>-8.9352891362541698</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-9.8645119362814118</c:v>
+                  <c:v>-9.9112783872395216</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1835,67 +1832,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-24.825831217445973</c:v>
+                  <c:v>-23.82813296867765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-24.42856265433311</c:v>
+                  <c:v>-23.519433521775909</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-24.011354271477963</c:v>
+                  <c:v>-23.19375952853526</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-23.574546593420266</c:v>
+                  <c:v>-22.851284810475221</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-23.118496141600239</c:v>
+                  <c:v>-22.492192156142416</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-22.643575143366586</c:v>
+                  <c:v>-22.116673223551054</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-22.150171228165355</c:v>
+                  <c:v>-21.724928437889609</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-21.63868711115769</c:v>
+                  <c:v>-21.317166884548143</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-21.109540264524604</c:v>
+                  <c:v>-20.893606197523482</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20.563162576727148</c:v>
+                  <c:v>-20.454472443261693</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-19.420512186366274</c:v>
+                  <c:v>-19.53043143267238</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-18.825172112470568</c:v>
+                  <c:v>-19.046017363445763</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-18.2144656935365</c:v>
+                  <c:v>-18.547016337955782</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-17.58889138676383</c:v>
+                  <c:v>-18.033694687313591</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-16.94895978448875</c:v>
+                  <c:v>-17.506326385957379</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-16.29519319743962</c:v>
+                  <c:v>-16.965192905424296</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-15.628125228428157</c:v>
+                  <c:v>-16.410583064121127</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-14.94830033682395</c:v>
+                  <c:v>-15.842792873173584</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-14.256273394168016</c:v>
+                  <c:v>-15.262125378436776</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-13.552609231287864</c:v>
+                  <c:v>-14.668890498750928</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1907,67 +1904,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-13.552230206388673</c:v>
+                  <c:v>-12.992055089910252</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-14.255925571613801</c:v>
+                  <c:v>-13.730417435430004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-14.94798528258711</c:v>
+                  <c:v>-14.461451464682787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-15.627844481735664</c:v>
+                  <c:v>-15.184767003910704</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-16.294948269516723</c:v>
+                  <c:v>-15.899977998934611</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-16.948752157325458</c:v>
+                  <c:v>-16.606702721202282</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-17.588722511905392</c:v>
+                  <c:v>-17.304563971527834</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-18.214336990898609</c:v>
+                  <c:v>-17.993189281413734</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-18.825084969180441</c:v>
+                  <c:v>-18.67221111184783</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-19.420467955630489</c:v>
+                  <c:v>-19.341267049469508</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-20</c:v>
+                  <c:v>-20.000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-20.563208089543348</c:v>
+                  <c:v>-20.648058378833856</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-21.109632535089961</c:v>
+                  <c:v>-21.285096298689638</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-21.638827346241598</c:v>
+                  <c:v>-21.910773754219893</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-22.150360595388669</c:v>
+                  <c:v>-22.524756803481743</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-22.643814770248621</c:v>
+                  <c:v>-23.126717746171163</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-23.118787114638501</c:v>
+                  <c:v>-23.716335298526101</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-23.574889957203627</c:v>
+                  <c:v>-24.293294764804742</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-24.011751027834091</c:v>
+                  <c:v>-24.857288205247652</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-24.429013761510788</c:v>
+                  <c:v>-25.408014600434004</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-24.826337589332955</c:v>
+                  <c:v>-25.945180011944267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1987,67 +1984,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>13.552736578275663</c:v>
+                  <c:v>15.109102133176851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.256376678791474</c:v>
+                  <c:v>15.618998514088089</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.948382038943242</c:v>
+                  <c:v>16.124980141395174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.628187845519026</c:v>
+                  <c:v>16.626776958240217</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.295239242554977</c:v>
+                  <c:v>17.124121141318291</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.948991784207493</c:v>
+                  <c:v>17.616747243822388</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.588911879128705</c:v>
+                  <c:v>18.104392337119965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.21447722598252</c:v>
+                  <c:v>18.586796151085473</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.825177239745798</c:v>
+                  <c:v>19.063701213013974</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.420513468446686</c:v>
+                  <c:v>19.53485298504166</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.563163858807567</c:v>
+                  <c:v>20.458893995630973</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.109545391799841</c:v>
+                  <c:v>20.911290047091697</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.638698643603707</c:v>
+                  <c:v>21.356946697677845</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.150191720530227</c:v>
+                  <c:v>21.795626087695972</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.64360714308533</c:v>
+                  <c:v>22.227094081416055</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.118542186715594</c:v>
+                  <c:v>22.651120392036404</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.574609210511134</c:v>
+                  <c:v>23.067478704594315</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.011435973597251</c:v>
+                  <c:v>23.475946796756844</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.428665938956573</c:v>
+                  <c:v>23.876306657427222</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24.825958564433762</c:v>
+                  <c:v>24.268344603103579</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2059,67 +2056,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-24.825452192546781</c:v>
+                  <c:v>-22.151297559836966</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-24.428214831778899</c:v>
+                  <c:v>-21.98772557876913</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-24.011039217241123</c:v>
+                  <c:v>-21.812418120044455</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-23.574265846727776</c:v>
+                  <c:v>-21.625468750264794</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-23.118251213677333</c:v>
+                  <c:v>-21.426977249652715</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-22.643367516203291</c:v>
+                  <c:v>-21.217049558795946</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-22.150002353306913</c:v>
+                  <c:v>-20.995797722103841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-21.638558408519799</c:v>
+                  <c:v>-20.763339828006092</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-21.10945312123448</c:v>
+                  <c:v>-20.519799945925545</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-20.563118345991366</c:v>
+                  <c:v>-20.265308060058818</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-19.420557699182467</c:v>
+                  <c:v>-19.724017368244535</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-18.825264383035922</c:v>
+                  <c:v>-19.437507464611908</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-18.214605928620411</c:v>
+                  <c:v>-19.140623207627524</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-17.589080753987144</c:v>
+                  <c:v>-18.833523052905722</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-16.949199411370785</c:v>
+                  <c:v>-18.516370908577485</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-16.295484170477884</c:v>
+                  <c:v>-18.189336047807981</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-15.628468592211515</c:v>
+                  <c:v>-17.852593018450641</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-14.948697093180078</c:v>
+                  <c:v>-17.506321549885975</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-14.256724501345689</c:v>
+                  <c:v>-17.150706457094863</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-13.553115603174851</c:v>
+                  <c:v>-16.785937542017532</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2139,67 +2136,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>33.581310494750326</c:v>
+                  <c:v>34.29018653133565</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.849373558795747</c:v>
+                  <c:v>34.424564599206647</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.089810122678202</c:v>
+                  <c:v>34.544990845299921</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>34.302423942617317</c:v>
+                  <c:v>34.651400994685552</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.487041483693488</c:v>
+                  <c:v>34.743738253225104</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>34.643512061486689</c:v>
+                  <c:v>34.821953337884253</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.771707965064742</c:v>
+                  <c:v>34.886004503036553</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34.871524561220696</c:v>
+                  <c:v>34.93585756274426</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.942880379874225</c:v>
+                  <c:v>34.971485909004379</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.985717180567313</c:v>
+                  <c:v>34.992870525950067</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.985717180567313</c:v>
+                  <c:v>34.992870525950067</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.942880379874225</c:v>
+                  <c:v>34.971485909004379</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.871524561220696</c:v>
+                  <c:v>34.93585756274426</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.771707965064742</c:v>
+                  <c:v>34.886004503036553</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.643512061486689</c:v>
+                  <c:v>34.821953337884253</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>34.487041483693488</c:v>
+                  <c:v>34.743738253225104</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>34.302423942617317</c:v>
+                  <c:v>34.651400994685552</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34.089810122678202</c:v>
+                  <c:v>34.544990845299921</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33.849373558795747</c:v>
+                  <c:v>34.424564599206647</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>33.581310494750326</c:v>
+                  <c:v>34.29018653133565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2211,67 +2208,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>-9.8636265394952538</c:v>
+                  <c:v>-6.1173959351322393</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8.9003536377785153</c:v>
+                  <c:v>-5.5150001145893084</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-7.9298162875257772</c:v>
+                  <c:v>-4.909660780839868</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-6.9528066391301708</c:v>
+                  <c:v>-4.3017010207898609</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-5.9701221256599553</c:v>
+                  <c:v>-3.6914453199416575</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-4.9825648119954424</c:v>
+                  <c:v>-3.0792193892068549</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.9909407401854571</c:v>
+                  <c:v>-2.4653499910650627</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2.996059271557638</c:v>
+                  <c:v>-1.8501647651614226</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-1.9987324261195467</c:v>
+                  <c:v>-1.2339920534359656</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.99977421978977865</c:v>
+                  <c:v>-0.61716072487813445</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.99977421978977976</c:v>
+                  <c:v>0.61716072487813523</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9987324261195467</c:v>
+                  <c:v>1.2339920534359656</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.996059271557638</c:v>
+                  <c:v>1.8501647651614226</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.9909407401854557</c:v>
+                  <c:v>2.4653499910650618</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.9825648119954424</c:v>
+                  <c:v>3.0792193892068549</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.9701221256599561</c:v>
+                  <c:v>3.6914453199416584</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.9528066391301708</c:v>
+                  <c:v>4.3017010207898609</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.9298162875257772</c:v>
+                  <c:v>4.909660780839868</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.9003536377785153</c:v>
+                  <c:v>5.5150001145893075</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.8636265394952538</c:v>
+                  <c:v>6.1173959351322393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2291,67 +2288,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>24.825958564433762</c:v>
+                  <c:v>24.268344603103579</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.428665938956573</c:v>
+                  <c:v>23.876306657427222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.011435973597251</c:v>
+                  <c:v>23.475946796756844</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.574609210511134</c:v>
+                  <c:v>23.067478704594315</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.118542186715594</c:v>
+                  <c:v>22.6511203920364</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.64360714308533</c:v>
+                  <c:v>22.227094081416055</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.150191720530227</c:v>
+                  <c:v>21.795626087695972</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.638698643603707</c:v>
+                  <c:v>21.356946697677845</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21.109545391799841</c:v>
+                  <c:v>20.911290047091697</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.563163858807567</c:v>
+                  <c:v>20.458893995630973</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>19.420513468446686</c:v>
+                  <c:v>19.53485298504166</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.825177239745798</c:v>
+                  <c:v>19.063701213013974</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.21447722598252</c:v>
+                  <c:v>18.586796151085473</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17.588911879128705</c:v>
+                  <c:v>18.104392337119965</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16.948991784207493</c:v>
+                  <c:v>17.616747243822388</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.295239242554977</c:v>
+                  <c:v>17.124121141318291</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.628187845519026</c:v>
+                  <c:v>16.626776958240217</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.948382038943242</c:v>
+                  <c:v>16.124980141395174</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.256376678791474</c:v>
+                  <c:v>15.618998514088089</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13.552736578275663</c:v>
+                  <c:v>15.109102133176851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2363,67 +2360,67 @@
                 <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>13.553115603174851</c:v>
+                  <c:v>16.785937542017532</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.256724501345689</c:v>
+                  <c:v>17.150706457094863</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.948697093180078</c:v>
+                  <c:v>17.506321549885975</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.628468592211515</c:v>
+                  <c:v>17.852593018450641</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.295484170477884</c:v>
+                  <c:v>18.189336047807984</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.949199411370785</c:v>
+                  <c:v>18.516370908577485</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.589080753987144</c:v>
+                  <c:v>18.833523052905722</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.214605928620411</c:v>
+                  <c:v>19.140623207627524</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.825264383035922</c:v>
+                  <c:v>19.437507464611908</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>19.420557699182467</c:v>
+                  <c:v>19.724017368244535</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.563118345991366</c:v>
+                  <c:v>20.265308060058818</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.10945312123448</c:v>
+                  <c:v>20.519799945925545</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.638558408519799</c:v>
+                  <c:v>20.763339828006092</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.150002353306913</c:v>
+                  <c:v>20.995797722103841</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.643367516203291</c:v>
+                  <c:v>21.217049558795946</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.118251213677333</c:v>
+                  <c:v>21.426977249652715</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.574265846727776</c:v>
+                  <c:v>21.625468750264794</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24.011039217241123</c:v>
+                  <c:v>21.812418120044455</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>24.428214831778899</c:v>
+                  <c:v>21.98772557876913</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>24.825452192546781</c:v>
+                  <c:v>22.151297559836966</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2443,7 +2440,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5707963300245439E-3</c:v>
+                  <c:v>8.2842712474619002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2485,37 +2482,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.5707963300245439E-3</c:v>
+                  <c:v>8.2842712474619002</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5707963300245439E-3</c:v>
+                  <c:v>8.2842712474619002</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5707963300245439E-3</c:v>
+                  <c:v>8.2842712474619002</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5707963300245439E-3</c:v>
+                  <c:v>8.2842712474619002</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5707963300245439E-3</c:v>
+                  <c:v>8.2842712474619002</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5707963300245439E-3</c:v>
+                  <c:v>8.2842712474619002</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>20</c:v>
@@ -2578,11 +2575,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="182991872"/>
-        <c:axId val="183010048"/>
+        <c:axId val="165170560"/>
+        <c:axId val="165188736"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="182991872"/>
+        <c:axId val="165170560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -2613,13 +2610,13 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="183010048"/>
+        <c:crossAx val="165188736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183010048"/>
+        <c:axId val="165188736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -2659,7 +2656,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="182991872"/>
+        <c:crossAx val="165170560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
@@ -2843,11 +2840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="176659072"/>
-        <c:axId val="183014912"/>
+        <c:axId val="165192832"/>
+        <c:axId val="165194368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="176659072"/>
+        <c:axId val="165192832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,12 +2853,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183014912"/>
+        <c:crossAx val="165194368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="183014912"/>
+        <c:axId val="165194368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2872,7 +2869,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="176659072"/>
+        <c:crossAx val="165192832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2961,204 +2958,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Лист1"/>
-      <sheetName val="Лист2"/>
-      <sheetName val="Лист3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="D3">
-            <v>1999</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>1636.6427754028862</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>1339.9697720252429</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>1097.0744605519587</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>898.20859927032609</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>735.39100290171325</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>602.08722961249202</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>492.94733091927139</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>403.59113947131624</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>330.43247755495156</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>270.53523118998879</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>221.49551356630545</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>181.3451886255356</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>148.47288285045346</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17">
-            <v>121.55931518781071</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18">
-            <v>99.524349667360042</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19">
-            <v>81.483645752754072</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="D20">
-            <v>69.435782630532387</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="D21">
-            <v>69.435782630532387</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="D22">
-            <v>81.483645752754072</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="D23">
-            <v>99.524349667360042</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="D24">
-            <v>121.55931518781071</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="D25">
-            <v>148.47288285045346</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="D26">
-            <v>181.3451886255356</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="D27">
-            <v>221.49551356630545</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="D28">
-            <v>270.53523118998879</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="D29">
-            <v>330.43247755495156</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="D30">
-            <v>403.59113947131624</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="D31">
-            <v>492.94733091927139</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="D32">
-            <v>602.08722961249202</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="D33">
-            <v>735.39100290171325</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="D34">
-            <v>898.20859927032609</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="D35">
-            <v>1097.0744605519587</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="D36">
-            <v>1339.9697720252429</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="D37">
-            <v>1636.6427754028862</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="D38">
-            <v>1999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3761,7 +3560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3797,14 +3596,14 @@
       <c r="AB1" s="59"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B2" s="103" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="107">
-        <v>1.9999</v>
-      </c>
-      <c r="E2" s="108"/>
+      <c r="B2" s="145" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="146"/>
+      <c r="D2" s="149">
+        <v>1.5</v>
+      </c>
+      <c r="E2" s="150"/>
       <c r="O2" s="59"/>
       <c r="P2" s="59"/>
       <c r="Q2" s="59"/>
@@ -3821,14 +3620,14 @@
       <c r="AB2" s="59"/>
     </row>
     <row r="3" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="105" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="106"/>
-      <c r="D3" s="109">
+      <c r="B3" s="147" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="148"/>
+      <c r="D3" s="151">
         <v>20</v>
       </c>
-      <c r="E3" s="110"/>
+      <c r="E3" s="152"/>
       <c r="O3" s="59"/>
       <c r="P3" s="59"/>
       <c r="Q3" s="59"/>
@@ -3861,20 +3660,20 @@
       <c r="AB4" s="59"/>
     </row>
     <row r="5" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="115" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="116"/>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="117"/>
+      <c r="B5" s="157" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="158"/>
+      <c r="H5" s="158"/>
+      <c r="I5" s="158"/>
+      <c r="J5" s="158"/>
+      <c r="K5" s="158"/>
+      <c r="L5" s="158"/>
+      <c r="M5" s="159"/>
       <c r="N5" s="54"/>
       <c r="O5" s="51"/>
       <c r="P5" s="51"/>
@@ -3892,30 +3691,30 @@
       <c r="AB5" s="59"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="141" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="142"/>
+      <c r="D6" s="141" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="142"/>
+      <c r="F6" s="141" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="128"/>
-      <c r="D6" s="127" t="s">
+      <c r="G6" s="142"/>
+      <c r="H6" s="141" t="s">
         <v>42</v>
       </c>
-      <c r="E6" s="128"/>
-      <c r="F6" s="127" t="s">
+      <c r="I6" s="142"/>
+      <c r="J6" s="141" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="128"/>
-      <c r="H6" s="127" t="s">
+      <c r="K6" s="142"/>
+      <c r="L6" s="141" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="128"/>
-      <c r="J6" s="127" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="128"/>
-      <c r="L6" s="127" t="s">
-        <v>46</v>
-      </c>
-      <c r="M6" s="128"/>
+      <c r="M6" s="142"/>
       <c r="O6" s="59"/>
       <c r="P6" s="59"/>
       <c r="Q6" s="59"/>
@@ -4105,20 +3904,20 @@
       <c r="AB10" s="59"/>
     </row>
     <row r="11" spans="1:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="122" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="123"/>
-      <c r="M11" s="124"/>
+      <c r="B11" s="160" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="161"/>
+      <c r="D11" s="161"/>
+      <c r="E11" s="161"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="161"/>
+      <c r="K11" s="161"/>
+      <c r="L11" s="161"/>
+      <c r="M11" s="162"/>
       <c r="O11" s="59"/>
       <c r="P11" s="59"/>
       <c r="Q11" s="59"/>
@@ -4135,25 +3934,25 @@
       <c r="AB11" s="59"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="111" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="112"/>
-      <c r="E12" s="113">
+      <c r="B12" s="153" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="154"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="155">
         <f>TAN((2 - D2) * PI() / 4) * D3</f>
-        <v>1.5707963300245439E-3</v>
-      </c>
-      <c r="F12" s="114"/>
-      <c r="G12" s="132" t="s">
-        <v>48</v>
-      </c>
-      <c r="H12" s="133"/>
-      <c r="I12" s="133"/>
-      <c r="J12" s="133"/>
-      <c r="K12" s="133"/>
-      <c r="L12" s="133"/>
-      <c r="M12" s="134"/>
+        <v>8.2842712474619002</v>
+      </c>
+      <c r="F12" s="156"/>
+      <c r="G12" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="129"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
+      <c r="K12" s="129"/>
+      <c r="L12" s="129"/>
+      <c r="M12" s="130"/>
       <c r="O12" s="59"/>
       <c r="P12" s="59"/>
       <c r="Q12" s="59"/>
@@ -4170,25 +3969,25 @@
       <c r="AB12" s="59"/>
     </row>
     <row r="13" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="120" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="121"/>
-      <c r="D13" s="121"/>
-      <c r="E13" s="125">
+      <c r="B13" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="139">
         <f>SQRT((E12-C7)^2+C9^2)</f>
-        <v>28.285381990006819</v>
-      </c>
-      <c r="F13" s="126"/>
-      <c r="G13" s="140" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="141"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="141"/>
-      <c r="K13" s="141"/>
-      <c r="L13" s="141"/>
-      <c r="M13" s="142"/>
+        <v>34.641016151377549</v>
+      </c>
+      <c r="F13" s="140"/>
+      <c r="G13" s="136" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" s="137"/>
+      <c r="I13" s="137"/>
+      <c r="J13" s="137"/>
+      <c r="K13" s="137"/>
+      <c r="L13" s="137"/>
+      <c r="M13" s="138"/>
       <c r="O13" s="59"/>
       <c r="P13" s="59"/>
       <c r="Q13" s="59"/>
@@ -4205,23 +4004,23 @@
       <c r="AB13" s="59"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="120" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="121"/>
-      <c r="D14" s="121"/>
-      <c r="E14" s="125">
+      <c r="B14" s="115" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="139">
         <f>SQRT((E12-E7)^2+E9^2)</f>
-        <v>35.001570796330022</v>
-      </c>
-      <c r="F14" s="126"/>
-      <c r="G14" s="140"/>
-      <c r="H14" s="141"/>
-      <c r="I14" s="141"/>
-      <c r="J14" s="141"/>
-      <c r="K14" s="141"/>
-      <c r="L14" s="141"/>
-      <c r="M14" s="142"/>
+        <v>43.284271247461902</v>
+      </c>
+      <c r="F14" s="140"/>
+      <c r="G14" s="136"/>
+      <c r="H14" s="137"/>
+      <c r="I14" s="137"/>
+      <c r="J14" s="137"/>
+      <c r="K14" s="137"/>
+      <c r="L14" s="137"/>
+      <c r="M14" s="138"/>
       <c r="O14" s="59"/>
       <c r="P14" s="59"/>
       <c r="Q14" s="59"/>
@@ -4238,23 +4037,23 @@
       <c r="AB14" s="59"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B15" s="120" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="121"/>
-      <c r="D15" s="121"/>
-      <c r="E15" s="125">
+      <c r="B15" s="115" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="139">
         <f>SQRT((E12-G7)^2+G9^2)</f>
-        <v>28.285381990006819</v>
-      </c>
-      <c r="F15" s="126"/>
-      <c r="G15" s="140"/>
-      <c r="H15" s="141"/>
-      <c r="I15" s="141"/>
-      <c r="J15" s="141"/>
-      <c r="K15" s="141"/>
-      <c r="L15" s="141"/>
-      <c r="M15" s="142"/>
+        <v>34.641016151377549</v>
+      </c>
+      <c r="F15" s="140"/>
+      <c r="G15" s="136"/>
+      <c r="H15" s="137"/>
+      <c r="I15" s="137"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="137"/>
+      <c r="L15" s="137"/>
+      <c r="M15" s="138"/>
       <c r="O15" s="59"/>
       <c r="P15" s="59"/>
       <c r="Q15" s="59"/>
@@ -4271,92 +4070,92 @@
       <c r="AB15" s="59"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="B16" s="120" t="s">
-        <v>68</v>
-      </c>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
-      <c r="E16" s="125">
+      <c r="B16" s="115" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
+      <c r="E16" s="139">
         <f>SQRT((E12-I7)^2+I9^2)</f>
-        <v>28.283160548534884</v>
-      </c>
-      <c r="F16" s="126"/>
-      <c r="G16" s="140"/>
-      <c r="H16" s="141"/>
-      <c r="I16" s="141"/>
-      <c r="J16" s="141"/>
-      <c r="K16" s="141"/>
-      <c r="L16" s="141"/>
-      <c r="M16" s="142"/>
+        <v>23.178833020733549</v>
+      </c>
+      <c r="F16" s="140"/>
+      <c r="G16" s="136"/>
+      <c r="H16" s="137"/>
+      <c r="I16" s="137"/>
+      <c r="J16" s="137"/>
+      <c r="K16" s="137"/>
+      <c r="L16" s="137"/>
+      <c r="M16" s="138"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B17" s="120" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="125">
+      <c r="B17" s="115" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="116"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="139">
         <f>SQRT((E12-K7)^2+K9^2)</f>
-        <v>34.998429203669978</v>
-      </c>
-      <c r="F17" s="126"/>
-      <c r="G17" s="140"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="141"/>
-      <c r="J17" s="141"/>
-      <c r="K17" s="141"/>
-      <c r="L17" s="141"/>
-      <c r="M17" s="142"/>
+        <v>26.715728752538098</v>
+      </c>
+      <c r="F17" s="140"/>
+      <c r="G17" s="136"/>
+      <c r="H17" s="137"/>
+      <c r="I17" s="137"/>
+      <c r="J17" s="137"/>
+      <c r="K17" s="137"/>
+      <c r="L17" s="137"/>
+      <c r="M17" s="138"/>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B18" s="120" t="s">
-        <v>70</v>
-      </c>
-      <c r="C18" s="121"/>
-      <c r="D18" s="121"/>
-      <c r="E18" s="125">
+      <c r="B18" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="116"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="139">
         <f>SQRT((E12-M7)^2+M9^2)</f>
-        <v>28.283160548534884</v>
-      </c>
-      <c r="F18" s="126"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="141"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="141"/>
-      <c r="K18" s="141"/>
-      <c r="L18" s="141"/>
-      <c r="M18" s="142"/>
+        <v>23.178833020733549</v>
+      </c>
+      <c r="F18" s="140"/>
+      <c r="G18" s="136"/>
+      <c r="H18" s="137"/>
+      <c r="I18" s="137"/>
+      <c r="J18" s="137"/>
+      <c r="K18" s="137"/>
+      <c r="L18" s="137"/>
+      <c r="M18" s="138"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B19" s="120" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="121"/>
-      <c r="D19" s="121"/>
+      <c r="B19" s="115" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
       <c r="E19" s="48">
         <f>ATAN2(-(E12-C7), C9)</f>
-        <v>2.3562337585585102</v>
+        <v>2.5261129449194057</v>
       </c>
       <c r="F19" s="57">
         <f t="shared" ref="F19:F24" si="0">DEGREES(E19)</f>
-        <v>135.00224991164964</v>
-      </c>
-      <c r="G19" s="145" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="146"/>
-      <c r="I19" s="146"/>
-      <c r="J19" s="146"/>
-      <c r="K19" s="146"/>
-      <c r="L19" s="146"/>
-      <c r="M19" s="147"/>
+        <v>144.73561031724535</v>
+      </c>
+      <c r="G19" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="106"/>
+      <c r="I19" s="106"/>
+      <c r="J19" s="106"/>
+      <c r="K19" s="106"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="107"/>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B20" s="120" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="121"/>
-      <c r="D20" s="121"/>
+      <c r="B20" s="115" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
       <c r="E20" s="48">
         <f>ATAN2(-(E12-E7), E9)</f>
         <v>3.1415926535897931</v>
@@ -4365,64 +4164,64 @@
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="G20" s="148"/>
-      <c r="H20" s="149"/>
-      <c r="I20" s="149"/>
-      <c r="J20" s="149"/>
-      <c r="K20" s="149"/>
-      <c r="L20" s="149"/>
-      <c r="M20" s="150"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="109"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="109"/>
+      <c r="M20" s="110"/>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B21" s="120" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="121"/>
-      <c r="D21" s="121"/>
+      <c r="B21" s="115" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
       <c r="E21" s="48">
         <f>ATAN2(-(E12-G7), G9)</f>
-        <v>-2.3562337585585102</v>
+        <v>-2.5261129449194057</v>
       </c>
       <c r="F21" s="57">
         <f t="shared" si="0"/>
-        <v>-135.00224991164964</v>
-      </c>
-      <c r="G21" s="148"/>
-      <c r="H21" s="149"/>
-      <c r="I21" s="149"/>
-      <c r="J21" s="149"/>
-      <c r="K21" s="149"/>
-      <c r="L21" s="149"/>
-      <c r="M21" s="150"/>
+        <v>-144.73561031724535</v>
+      </c>
+      <c r="G21" s="108"/>
+      <c r="H21" s="109"/>
+      <c r="I21" s="109"/>
+      <c r="J21" s="109"/>
+      <c r="K21" s="109"/>
+      <c r="L21" s="109"/>
+      <c r="M21" s="110"/>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B22" s="120" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
+      <c r="B22" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="116"/>
+      <c r="D22" s="116"/>
       <c r="E22" s="48">
         <f>ATAN2(-(E12-I7), I9)</f>
-        <v>-0.78543743484786499</v>
+        <v>-1.04089353704597</v>
       </c>
       <c r="F22" s="57">
         <f t="shared" si="0"/>
-        <v>-45.002250088364235</v>
-      </c>
-      <c r="G22" s="148"/>
-      <c r="H22" s="149"/>
-      <c r="I22" s="149"/>
-      <c r="J22" s="149"/>
-      <c r="K22" s="149"/>
-      <c r="L22" s="149"/>
-      <c r="M22" s="150"/>
+        <v>-59.638806595178281</v>
+      </c>
+      <c r="G22" s="108"/>
+      <c r="H22" s="109"/>
+      <c r="I22" s="109"/>
+      <c r="J22" s="109"/>
+      <c r="K22" s="109"/>
+      <c r="L22" s="109"/>
+      <c r="M22" s="110"/>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B23" s="120" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
+      <c r="B23" s="115" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
       <c r="E23" s="48">
         <f>ATAN2(-(E12-K7), K9)</f>
         <v>0</v>
@@ -4431,141 +4230,141 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="148"/>
-      <c r="H23" s="149"/>
-      <c r="I23" s="149"/>
-      <c r="J23" s="149"/>
-      <c r="K23" s="149"/>
-      <c r="L23" s="149"/>
-      <c r="M23" s="150"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="110"/>
     </row>
     <row r="24" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B24" s="120" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="121"/>
-      <c r="D24" s="121"/>
+      <c r="B24" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
       <c r="E24" s="48">
         <f>ATAN2(-(E12-M7), M9)</f>
-        <v>0.78543743484786499</v>
+        <v>1.04089353704597</v>
       </c>
       <c r="F24" s="57">
         <f t="shared" si="0"/>
-        <v>45.002250088364235</v>
-      </c>
-      <c r="G24" s="151"/>
-      <c r="H24" s="152"/>
-      <c r="I24" s="152"/>
-      <c r="J24" s="152"/>
-      <c r="K24" s="152"/>
-      <c r="L24" s="152"/>
-      <c r="M24" s="153"/>
+        <v>59.638806595178281</v>
+      </c>
+      <c r="G24" s="111"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="113"/>
     </row>
     <row r="25" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B25" s="118" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="119"/>
-      <c r="D25" s="119"/>
-      <c r="E25" s="161">
+      <c r="B25" s="143" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="144"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="123">
         <f>MAX(E13:F18)</f>
-        <v>35.001570796330022</v>
-      </c>
-      <c r="F25" s="162"/>
-      <c r="G25" s="129"/>
-      <c r="H25" s="130"/>
-      <c r="I25" s="130"/>
-      <c r="J25" s="130"/>
-      <c r="K25" s="130"/>
-      <c r="L25" s="130"/>
-      <c r="M25" s="131"/>
+        <v>43.284271247461902</v>
+      </c>
+      <c r="F25" s="124"/>
+      <c r="G25" s="125"/>
+      <c r="H25" s="126"/>
+      <c r="I25" s="126"/>
+      <c r="J25" s="126"/>
+      <c r="K25" s="126"/>
+      <c r="L25" s="126"/>
+      <c r="M25" s="127"/>
     </row>
     <row r="26" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="135" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
+      <c r="B26" s="131" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="132"/>
+      <c r="D26" s="132"/>
       <c r="E26" s="74">
         <f>SIGN(E12) * D3 / E25</f>
-        <v>0.5714029269251264</v>
+        <v>0.46206160860737044</v>
       </c>
       <c r="F26" s="75">
         <f>ABS(E26)</f>
-        <v>0.5714029269251264</v>
-      </c>
-      <c r="G26" s="137" t="s">
+        <v>0.46206160860737044</v>
+      </c>
+      <c r="G26" s="133" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26" s="134"/>
+      <c r="I26" s="134"/>
+      <c r="J26" s="134"/>
+      <c r="K26" s="134"/>
+      <c r="L26" s="134"/>
+      <c r="M26" s="135"/>
+    </row>
+    <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="114" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="114"/>
+      <c r="D29" s="114"/>
+      <c r="E29" s="114"/>
+      <c r="F29" s="114"/>
+      <c r="G29" s="114"/>
+      <c r="H29" s="114"/>
+      <c r="I29" s="114"/>
+      <c r="J29" s="114"/>
+      <c r="K29" s="114"/>
+      <c r="L29" s="114"/>
+      <c r="M29" s="114"/>
+      <c r="N29" s="114"/>
+      <c r="O29" s="114"/>
+      <c r="P29" s="114"/>
+      <c r="Q29" s="114"/>
+      <c r="R29" s="114"/>
+      <c r="S29" s="114"/>
+      <c r="T29" s="114"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="103" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="120" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="121"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="117" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="118"/>
+      <c r="H30" s="119"/>
+      <c r="I30" s="120" t="s">
+        <v>50</v>
+      </c>
+      <c r="J30" s="121"/>
+      <c r="K30" s="122"/>
+      <c r="L30" s="117" t="s">
         <v>51</v>
       </c>
-      <c r="H26" s="138"/>
-      <c r="I26" s="138"/>
-      <c r="J26" s="138"/>
-      <c r="K26" s="138"/>
-      <c r="L26" s="138"/>
-      <c r="M26" s="139"/>
-    </row>
-    <row r="29" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="154" t="s">
-        <v>73</v>
-      </c>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
-      <c r="G29" s="154"/>
-      <c r="H29" s="154"/>
-      <c r="I29" s="154"/>
-      <c r="J29" s="154"/>
-      <c r="K29" s="154"/>
-      <c r="L29" s="154"/>
-      <c r="M29" s="154"/>
-      <c r="N29" s="154"/>
-      <c r="O29" s="154"/>
-      <c r="P29" s="154"/>
-      <c r="Q29" s="154"/>
-      <c r="R29" s="154"/>
-      <c r="S29" s="154"/>
-      <c r="T29" s="154"/>
-    </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B30" s="143" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="158" t="s">
+      <c r="M30" s="118"/>
+      <c r="N30" s="119"/>
+      <c r="O30" s="120" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="159"/>
-      <c r="E30" s="160"/>
-      <c r="F30" s="155" t="s">
+      <c r="P30" s="121"/>
+      <c r="Q30" s="122"/>
+      <c r="R30" s="117" t="s">
         <v>53</v>
       </c>
-      <c r="G30" s="156"/>
-      <c r="H30" s="157"/>
-      <c r="I30" s="158" t="s">
-        <v>54</v>
-      </c>
-      <c r="J30" s="159"/>
-      <c r="K30" s="160"/>
-      <c r="L30" s="155" t="s">
-        <v>55</v>
-      </c>
-      <c r="M30" s="156"/>
-      <c r="N30" s="157"/>
-      <c r="O30" s="158" t="s">
-        <v>56</v>
-      </c>
-      <c r="P30" s="159"/>
-      <c r="Q30" s="160"/>
-      <c r="R30" s="155" t="s">
-        <v>57</v>
-      </c>
-      <c r="S30" s="156"/>
-      <c r="T30" s="157"/>
+      <c r="S30" s="118"/>
+      <c r="T30" s="119"/>
     </row>
     <row r="31" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="144"/>
+      <c r="B31" s="104"/>
       <c r="C31" s="62" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D31" s="63" t="s">
         <v>32</v>
@@ -4574,7 +4373,7 @@
         <v>35</v>
       </c>
       <c r="F31" s="68" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G31" s="69" t="s">
         <v>32</v>
@@ -4583,7 +4382,7 @@
         <v>35</v>
       </c>
       <c r="I31" s="62" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J31" s="63" t="s">
         <v>32</v>
@@ -4592,7 +4391,7 @@
         <v>35</v>
       </c>
       <c r="L31" s="68" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="M31" s="69" t="s">
         <v>32</v>
@@ -4601,7 +4400,7 @@
         <v>35</v>
       </c>
       <c r="O31" s="62" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P31" s="63" t="s">
         <v>32</v>
@@ -4610,7 +4409,7 @@
         <v>35</v>
       </c>
       <c r="R31" s="68" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="S31" s="69" t="s">
         <v>32</v>
@@ -4625,75 +4424,75 @@
       </c>
       <c r="C32" s="81">
         <f>($B32-0.5) * $E$26 + $E$19</f>
-        <v>2.0705322950959468</v>
+        <v>2.2950821406157207</v>
       </c>
       <c r="D32" s="82">
         <f>$E$12+$E$13*COS(C32)</f>
-        <v>-13.552609231287864</v>
+        <v>-14.668890498750928</v>
       </c>
       <c r="E32" s="83">
         <f>$E$13*SIN(C32)</f>
-        <v>24.826337589332955</v>
+        <v>25.945180011944267</v>
       </c>
       <c r="F32" s="84">
         <f>($B32 - 0.5) * $E$26 + $E$20</f>
-        <v>2.8558911901272301</v>
+        <v>2.9105618492861081</v>
       </c>
       <c r="G32" s="85">
         <f>$E$12+$E$14*COS(F32)</f>
-        <v>-33.58118314776253</v>
+        <v>-33.849974896909728</v>
       </c>
       <c r="H32" s="86">
         <f>$E$14*SIN(F32)</f>
-        <v>9.8645119362814189</v>
+        <v>9.9112783872395323</v>
       </c>
       <c r="I32" s="81">
         <f>($B32 - 0.5) * $E$26 + $E$21</f>
-        <v>-2.6419352220210737</v>
+        <v>-2.7571437492230908</v>
       </c>
       <c r="J32" s="82">
         <f>$E$12+$E$15*COS(I32)</f>
-        <v>-24.825831217445973</v>
+        <v>-23.82813296867765</v>
       </c>
       <c r="K32" s="83">
         <f>$E$15*SIN(I32)</f>
-        <v>-13.552230206388673</v>
+        <v>-12.992055089910252</v>
       </c>
       <c r="L32" s="84">
         <f xml:space="preserve"> ($B32 - 0.5) * $E$26 + $E$22</f>
-        <v>-1.0711388983104282</v>
+        <v>-1.2719243413496553</v>
       </c>
       <c r="M32" s="85">
         <f>$E$12+$E$16*COS(L32)</f>
-        <v>13.552736578275663</v>
+        <v>15.109102133176851</v>
       </c>
       <c r="N32" s="86">
         <f>$E$16*SIN(L32)</f>
-        <v>-24.825452192546781</v>
+        <v>-22.151297559836966</v>
       </c>
       <c r="O32" s="81">
         <f>($B32 - 0.5) * $E$26 + $E$23</f>
-        <v>-0.2857014634625632</v>
+        <v>-0.23103080430368522</v>
       </c>
       <c r="P32" s="82">
         <f>$E$12+$E$17*COS(O32)</f>
-        <v>33.581310494750326</v>
+        <v>34.29018653133565</v>
       </c>
       <c r="Q32" s="83">
         <f>$E$17*SIN(O32)</f>
-        <v>-9.8636265394952538</v>
+        <v>-6.1173959351322393</v>
       </c>
       <c r="R32" s="84">
         <f>($B32 - 0.5) * $E$26 + $E$24</f>
-        <v>0.49973597138530179</v>
+        <v>0.80986273274228471</v>
       </c>
       <c r="S32" s="85">
         <f>$E$12+$E$18*COS(R32)</f>
-        <v>24.825958564433762</v>
+        <v>24.268344603103579</v>
       </c>
       <c r="T32" s="86">
         <f>$E$18*SIN(R32)</f>
-        <v>13.553115603174851</v>
+        <v>16.785937542017532</v>
       </c>
     </row>
     <row r="33" spans="2:20" x14ac:dyDescent="0.25">
@@ -4702,75 +4501,75 @@
       </c>
       <c r="C33" s="65">
         <f t="shared" ref="C33:C52" si="1">($B33-0.5) * $E$26 + $E$19</f>
-        <v>2.0991024414422035</v>
+        <v>2.3181852210460892</v>
       </c>
       <c r="D33" s="66">
         <f t="shared" ref="D33:D52" si="2">$E$12+$E$13*COS(C33)</f>
-        <v>-14.256273394168016</v>
+        <v>-15.262125378436776</v>
       </c>
       <c r="E33" s="67">
         <f t="shared" ref="E33:E52" si="3">$E$13*SIN(C33)</f>
-        <v>24.429013761510788</v>
+        <v>25.408014600434004</v>
       </c>
       <c r="F33" s="71">
         <f t="shared" ref="F33:F52" si="4">($B33 - 0.5) * $E$26 + $E$20</f>
-        <v>2.8844613364734863</v>
+        <v>2.9336649297164765</v>
       </c>
       <c r="G33" s="72">
         <f t="shared" ref="G33:G52" si="5">$E$12+$E$14*COS(F33)</f>
-        <v>-33.849270274172284</v>
+        <v>-34.067691463555342</v>
       </c>
       <c r="H33" s="73">
         <f t="shared" ref="H33:H52" si="6">$E$14*SIN(F33)</f>
-        <v>8.9011525675104046</v>
+        <v>8.9352891362541804</v>
       </c>
       <c r="I33" s="65">
         <f t="shared" ref="I33:I52" si="7">($B33 - 0.5) * $E$26 + $E$21</f>
-        <v>-2.613365075674817</v>
+        <v>-2.7340406687927223</v>
       </c>
       <c r="J33" s="66">
         <f t="shared" ref="J33:J52" si="8">$E$12+$E$15*COS(I33)</f>
-        <v>-24.42856265433311</v>
+        <v>-23.519433521775909</v>
       </c>
       <c r="K33" s="67">
         <f t="shared" ref="K33:K52" si="9">$E$15*SIN(I33)</f>
-        <v>-14.255925571613801</v>
+        <v>-13.730417435430004</v>
       </c>
       <c r="L33" s="71">
         <f t="shared" ref="L33:L52" si="10" xml:space="preserve"> ($B33 - 0.5) * $E$26 + $E$22</f>
-        <v>-1.042568751964172</v>
+        <v>-1.2488212609192866</v>
       </c>
       <c r="M33" s="72">
         <f t="shared" ref="M33:M52" si="11">$E$12+$E$16*COS(L33)</f>
-        <v>14.256376678791474</v>
+        <v>15.618998514088089</v>
       </c>
       <c r="N33" s="73">
         <f t="shared" ref="N33:N52" si="12">$E$16*SIN(L33)</f>
-        <v>-24.428214831778899</v>
+        <v>-21.98772557876913</v>
       </c>
       <c r="O33" s="65">
         <f t="shared" ref="O33:O52" si="13">($B33 - 0.5) * $E$26 + $E$23</f>
-        <v>-0.25713131711630688</v>
+        <v>-0.20792772387331671</v>
       </c>
       <c r="P33" s="66">
         <f t="shared" ref="P33:P52" si="14">$E$12+$E$17*COS(O33)</f>
-        <v>33.849373558795747</v>
+        <v>34.424564599206647</v>
       </c>
       <c r="Q33" s="67">
         <f t="shared" ref="Q33:Q52" si="15">$E$17*SIN(O33)</f>
-        <v>-8.9003536377785153</v>
+        <v>-5.5150001145893084</v>
       </c>
       <c r="R33" s="71">
         <f t="shared" ref="R33:R52" si="16">($B33 - 0.5) * $E$26 + $E$24</f>
-        <v>0.52830611773155811</v>
+        <v>0.83296581317265328</v>
       </c>
       <c r="S33" s="72">
         <f t="shared" ref="S33:S52" si="17">$E$12+$E$18*COS(R33)</f>
-        <v>24.428665938956573</v>
+        <v>23.876306657427222</v>
       </c>
       <c r="T33" s="73">
         <f t="shared" ref="T33:T52" si="18">$E$18*SIN(R33)</f>
-        <v>14.256724501345689</v>
+        <v>17.150706457094863</v>
       </c>
     </row>
     <row r="34" spans="2:20" x14ac:dyDescent="0.25">
@@ -4779,75 +4578,75 @@
       </c>
       <c r="C34" s="65">
         <f t="shared" si="1"/>
-        <v>2.1276725877884597</v>
+        <v>2.3412883014764576</v>
       </c>
       <c r="D34" s="66">
         <f t="shared" si="2"/>
-        <v>-14.94830033682395</v>
+        <v>-15.842792873173584</v>
       </c>
       <c r="E34" s="67">
         <f t="shared" si="3"/>
-        <v>24.011751027834091</v>
+        <v>24.857288205247652</v>
       </c>
       <c r="F34" s="71">
         <f t="shared" si="4"/>
-        <v>2.9130314828197426</v>
+        <v>2.956768010146845</v>
       </c>
       <c r="G34" s="72">
         <f t="shared" si="5"/>
-        <v>-34.089728420558906</v>
+        <v>-34.26280357707833</v>
       </c>
       <c r="H34" s="73">
         <f t="shared" si="6"/>
-        <v>7.9305280981187476</v>
+        <v>7.9545308660430658</v>
       </c>
       <c r="I34" s="65">
         <f t="shared" si="7"/>
-        <v>-2.5847949293285608</v>
+        <v>-2.7109375883623539</v>
       </c>
       <c r="J34" s="66">
         <f t="shared" si="8"/>
-        <v>-24.011354271477963</v>
+        <v>-23.19375952853526</v>
       </c>
       <c r="K34" s="67">
         <f t="shared" si="9"/>
-        <v>-14.94798528258711</v>
+        <v>-14.461451464682787</v>
       </c>
       <c r="L34" s="71">
         <f t="shared" si="10"/>
-        <v>-1.0139986056179155</v>
+        <v>-1.2257181804889181</v>
       </c>
       <c r="M34" s="72">
         <f t="shared" si="11"/>
-        <v>14.948382038943242</v>
+        <v>16.124980141395174</v>
       </c>
       <c r="N34" s="73">
         <f t="shared" si="12"/>
-        <v>-24.011039217241123</v>
+        <v>-21.812418120044455</v>
       </c>
       <c r="O34" s="65">
         <f t="shared" si="13"/>
-        <v>-0.22856117077005056</v>
+        <v>-0.18482464344294819</v>
       </c>
       <c r="P34" s="66">
         <f t="shared" si="14"/>
-        <v>34.089810122678202</v>
+        <v>34.544990845299921</v>
       </c>
       <c r="Q34" s="67">
         <f t="shared" si="15"/>
-        <v>-7.9298162875257772</v>
+        <v>-4.909660780839868</v>
       </c>
       <c r="R34" s="71">
         <f t="shared" si="16"/>
-        <v>0.55687626407781443</v>
+        <v>0.85606889360302185</v>
       </c>
       <c r="S34" s="72">
         <f t="shared" si="17"/>
-        <v>24.011435973597251</v>
+        <v>23.475946796756844</v>
       </c>
       <c r="T34" s="73">
         <f t="shared" si="18"/>
-        <v>14.948697093180078</v>
+        <v>17.506321549885975</v>
       </c>
     </row>
     <row r="35" spans="2:20" x14ac:dyDescent="0.25">
@@ -4856,75 +4655,75 @@
       </c>
       <c r="C35" s="65">
         <f t="shared" si="1"/>
-        <v>2.1562427341347159</v>
+        <v>2.3643913819068261</v>
       </c>
       <c r="D35" s="66">
         <f t="shared" si="2"/>
-        <v>-15.628125228428157</v>
+        <v>-16.410583064121127</v>
       </c>
       <c r="E35" s="67">
         <f t="shared" si="3"/>
-        <v>23.574889957203627</v>
+        <v>24.293294764804742</v>
       </c>
       <c r="F35" s="71">
         <f t="shared" si="4"/>
-        <v>2.9416016291659988</v>
+        <v>2.9798710905772134</v>
       </c>
       <c r="G35" s="72">
         <f t="shared" si="5"/>
-        <v>-34.302361325526448</v>
+        <v>-34.435207100566458</v>
       </c>
       <c r="H35" s="73">
         <f t="shared" si="6"/>
-        <v>6.9534307496060261</v>
+        <v>6.9695270353298122</v>
       </c>
       <c r="I35" s="65">
         <f t="shared" si="7"/>
-        <v>-2.5562247829823046</v>
+        <v>-2.6878345079319854</v>
       </c>
       <c r="J35" s="66">
         <f t="shared" si="8"/>
-        <v>-23.574546593420266</v>
+        <v>-22.851284810475221</v>
       </c>
       <c r="K35" s="67">
         <f t="shared" si="9"/>
-        <v>-15.627844481735664</v>
+        <v>-15.184767003910704</v>
       </c>
       <c r="L35" s="71">
         <f t="shared" si="10"/>
-        <v>-0.98542845927165923</v>
+        <v>-1.2026151000585497</v>
       </c>
       <c r="M35" s="72">
         <f t="shared" si="11"/>
-        <v>15.628187845519026</v>
+        <v>16.626776958240217</v>
       </c>
       <c r="N35" s="73">
         <f t="shared" si="12"/>
-        <v>-23.574265846727776</v>
+        <v>-21.625468750264794</v>
       </c>
       <c r="O35" s="65">
         <f t="shared" si="13"/>
-        <v>-0.19999102442379424</v>
+        <v>-0.16172156301257964</v>
       </c>
       <c r="P35" s="66">
         <f t="shared" si="14"/>
-        <v>34.302423942617317</v>
+        <v>34.651400994685552</v>
       </c>
       <c r="Q35" s="67">
         <f t="shared" si="15"/>
-        <v>-6.9528066391301708</v>
+        <v>-4.3017010207898609</v>
       </c>
       <c r="R35" s="71">
         <f t="shared" si="16"/>
-        <v>0.58544641042407075</v>
+        <v>0.87917197403339031</v>
       </c>
       <c r="S35" s="72">
         <f t="shared" si="17"/>
-        <v>23.574609210511134</v>
+        <v>23.067478704594315</v>
       </c>
       <c r="T35" s="73">
         <f t="shared" si="18"/>
-        <v>15.628468592211515</v>
+        <v>17.852593018450641</v>
       </c>
     </row>
     <row r="36" spans="2:20" x14ac:dyDescent="0.25">
@@ -4933,75 +4732,75 @@
       </c>
       <c r="C36" s="65">
         <f t="shared" si="1"/>
-        <v>2.1848128804809726</v>
+        <v>2.3874944623371945</v>
       </c>
       <c r="D36" s="66">
         <f t="shared" si="2"/>
-        <v>-16.295193197439634</v>
+        <v>-16.965192905424296</v>
       </c>
       <c r="E36" s="67">
         <f t="shared" si="3"/>
-        <v>23.118787114638497</v>
+        <v>23.716335298526101</v>
       </c>
       <c r="F36" s="71">
         <f t="shared" si="4"/>
-        <v>2.970171775512255</v>
+        <v>3.0029741710075819</v>
       </c>
       <c r="G36" s="72">
         <f t="shared" si="5"/>
-        <v>-34.486995438578141</v>
+        <v>-34.584810017331115</v>
       </c>
       <c r="H36" s="73">
         <f t="shared" si="6"/>
-        <v>5.9706580266211331</v>
+        <v>5.9808033688150415</v>
       </c>
       <c r="I36" s="65">
         <f t="shared" si="7"/>
-        <v>-2.5276546366360479</v>
+        <v>-2.664731427501617</v>
       </c>
       <c r="J36" s="66">
         <f t="shared" si="8"/>
-        <v>-23.118496141600239</v>
+        <v>-22.492192156142416</v>
       </c>
       <c r="K36" s="67">
         <f t="shared" si="9"/>
-        <v>-16.294948269516723</v>
+        <v>-15.899977998934611</v>
       </c>
       <c r="L36" s="71">
         <f t="shared" si="10"/>
-        <v>-0.95685831292540291</v>
+        <v>-1.1795120196281812</v>
       </c>
       <c r="M36" s="72">
         <f t="shared" si="11"/>
-        <v>16.295239242554977</v>
+        <v>17.124121141318291</v>
       </c>
       <c r="N36" s="73">
         <f t="shared" si="12"/>
-        <v>-23.118251213677333</v>
+        <v>-21.426977249652715</v>
       </c>
       <c r="O36" s="65">
         <f t="shared" si="13"/>
-        <v>-0.17142087807753792</v>
+        <v>-0.13861848258221113</v>
       </c>
       <c r="P36" s="66">
         <f t="shared" si="14"/>
-        <v>34.487041483693488</v>
+        <v>34.743738253225104</v>
       </c>
       <c r="Q36" s="67">
         <f t="shared" si="15"/>
-        <v>-5.9701221256599553</v>
+        <v>-3.6914453199416575</v>
       </c>
       <c r="R36" s="71">
         <f t="shared" si="16"/>
-        <v>0.61401655677032707</v>
+        <v>0.90227505446375889</v>
       </c>
       <c r="S36" s="72">
         <f t="shared" si="17"/>
-        <v>23.118542186715594</v>
+        <v>22.6511203920364</v>
       </c>
       <c r="T36" s="73">
         <f t="shared" si="18"/>
-        <v>16.295484170477884</v>
+        <v>18.189336047807984</v>
       </c>
     </row>
     <row r="37" spans="2:20" x14ac:dyDescent="0.25">
@@ -5010,75 +4809,75 @@
       </c>
       <c r="C37" s="65">
         <f t="shared" si="1"/>
-        <v>2.2133830268272288</v>
+        <v>2.410597542767563</v>
       </c>
       <c r="D37" s="66">
         <f t="shared" si="2"/>
-        <v>-16.94895978448875</v>
+        <v>-17.506326385957379</v>
       </c>
       <c r="E37" s="67">
         <f t="shared" si="3"/>
-        <v>22.643814770248621</v>
+        <v>23.126717746171163</v>
       </c>
       <c r="F37" s="71">
         <f t="shared" si="4"/>
-        <v>2.9987419218585116</v>
+        <v>3.0260772514379504</v>
       </c>
       <c r="G37" s="72">
         <f t="shared" si="5"/>
-        <v>-34.643480061767946</v>
+        <v>-34.711532480019251</v>
       </c>
       <c r="H37" s="73">
         <f t="shared" si="6"/>
-        <v>4.9830120660407724</v>
+        <v>4.9888875765820719</v>
       </c>
       <c r="I37" s="65">
         <f t="shared" si="7"/>
-        <v>-2.4990844902897917</v>
+        <v>-2.6416283470712485</v>
       </c>
       <c r="J37" s="66">
         <f t="shared" si="8"/>
-        <v>-22.643575143366586</v>
+        <v>-22.116673223551054</v>
       </c>
       <c r="K37" s="67">
         <f t="shared" si="9"/>
-        <v>-16.948752157325458</v>
+        <v>-16.606702721202282</v>
       </c>
       <c r="L37" s="71">
         <f t="shared" si="10"/>
-        <v>-0.92828816657914659</v>
+        <v>-1.1564089391978125</v>
       </c>
       <c r="M37" s="72">
         <f t="shared" si="11"/>
-        <v>16.948991784207493</v>
+        <v>17.616747243822388</v>
       </c>
       <c r="N37" s="73">
         <f t="shared" si="12"/>
-        <v>-22.643367516203291</v>
+        <v>-21.217049558795946</v>
       </c>
       <c r="O37" s="65">
         <f t="shared" si="13"/>
-        <v>-0.1428507317312816</v>
+        <v>-0.11551540215184261</v>
       </c>
       <c r="P37" s="66">
         <f t="shared" si="14"/>
-        <v>34.643512061486689</v>
+        <v>34.821953337884253</v>
       </c>
       <c r="Q37" s="67">
         <f t="shared" si="15"/>
-        <v>-4.9825648119954424</v>
+        <v>-3.0792193892068549</v>
       </c>
       <c r="R37" s="71">
         <f t="shared" si="16"/>
-        <v>0.64258670311658339</v>
+        <v>0.92537813489412735</v>
       </c>
       <c r="S37" s="72">
         <f t="shared" si="17"/>
-        <v>22.64360714308533</v>
+        <v>22.227094081416055</v>
       </c>
       <c r="T37" s="73">
         <f t="shared" si="18"/>
-        <v>16.949199411370785</v>
+        <v>18.516370908577485</v>
       </c>
     </row>
     <row r="38" spans="2:20" x14ac:dyDescent="0.25">
@@ -5087,75 +4886,75 @@
       </c>
       <c r="C38" s="65">
         <f t="shared" si="1"/>
-        <v>2.241953173173485</v>
+        <v>2.4337006231979315</v>
       </c>
       <c r="D38" s="66">
         <f t="shared" si="2"/>
-        <v>-17.58889138676383</v>
+        <v>-18.033694687313591</v>
       </c>
       <c r="E38" s="67">
         <f t="shared" si="3"/>
-        <v>22.150360595388669</v>
+        <v>22.524756803481743</v>
       </c>
       <c r="F38" s="71">
         <f t="shared" si="4"/>
-        <v>3.0273120682047678</v>
+        <v>3.0491803318683188</v>
       </c>
       <c r="G38" s="72">
         <f t="shared" si="5"/>
-        <v>-34.771687472699867</v>
+        <v>-34.815306853230183</v>
       </c>
       <c r="H38" s="73">
         <f t="shared" si="6"/>
-        <v>3.9912989822672147</v>
+        <v>3.9943090724429657</v>
       </c>
       <c r="I38" s="65">
         <f t="shared" si="7"/>
-        <v>-2.4705143439435355</v>
+        <v>-2.61852526664088</v>
       </c>
       <c r="J38" s="66">
         <f t="shared" si="8"/>
-        <v>-22.150171228165355</v>
+        <v>-21.724928437889609</v>
       </c>
       <c r="K38" s="67">
         <f t="shared" si="9"/>
-        <v>-17.588722511905392</v>
+        <v>-17.304563971527834</v>
       </c>
       <c r="L38" s="71">
         <f t="shared" si="10"/>
-        <v>-0.89971802023289027</v>
+        <v>-1.1333058587674441</v>
       </c>
       <c r="M38" s="72">
         <f t="shared" si="11"/>
-        <v>17.588911879128705</v>
+        <v>18.104392337119965</v>
       </c>
       <c r="N38" s="73">
         <f t="shared" si="12"/>
-        <v>-22.150002353306913</v>
+        <v>-20.995797722103841</v>
       </c>
       <c r="O38" s="65">
         <f t="shared" si="13"/>
-        <v>-0.11428058538502528</v>
+        <v>-9.2412321721474094E-2</v>
       </c>
       <c r="P38" s="66">
         <f t="shared" si="14"/>
-        <v>34.771707965064742</v>
+        <v>34.886004503036553</v>
       </c>
       <c r="Q38" s="67">
         <f t="shared" si="15"/>
-        <v>-3.9909407401854571</v>
+        <v>-2.4653499910650627</v>
       </c>
       <c r="R38" s="71">
         <f t="shared" si="16"/>
-        <v>0.67115684946283971</v>
+        <v>0.94848121532449592</v>
       </c>
       <c r="S38" s="72">
         <f t="shared" si="17"/>
-        <v>22.150191720530227</v>
+        <v>21.795626087695972</v>
       </c>
       <c r="T38" s="73">
         <f t="shared" si="18"/>
-        <v>17.589080753987144</v>
+        <v>18.833523052905722</v>
       </c>
     </row>
     <row r="39" spans="2:20" x14ac:dyDescent="0.25">
@@ -5164,75 +4963,75 @@
       </c>
       <c r="C39" s="65">
         <f t="shared" si="1"/>
-        <v>2.2705233195197412</v>
+        <v>2.4568037036283004</v>
       </c>
       <c r="D39" s="66">
         <f t="shared" si="2"/>
-        <v>-18.2144656935365</v>
+        <v>-18.547016337955782</v>
       </c>
       <c r="E39" s="67">
         <f t="shared" si="3"/>
-        <v>21.638827346241598</v>
+        <v>21.910773754219893</v>
       </c>
       <c r="F39" s="71">
         <f t="shared" si="4"/>
-        <v>3.055882214551024</v>
+        <v>3.0722834122986877</v>
       </c>
       <c r="G39" s="72">
         <f t="shared" si="5"/>
-        <v>-34.871513028774679</v>
+        <v>-34.896077749614562</v>
       </c>
       <c r="H39" s="73">
         <f t="shared" si="6"/>
-        <v>2.9963282092794445</v>
+        <v>2.9975986913752215</v>
       </c>
       <c r="I39" s="65">
         <f t="shared" si="7"/>
-        <v>-2.4419441975972793</v>
+        <v>-2.5954221862105111</v>
       </c>
       <c r="J39" s="66">
         <f t="shared" si="8"/>
-        <v>-21.63868711115769</v>
+        <v>-21.317166884548143</v>
       </c>
       <c r="K39" s="67">
         <f t="shared" si="9"/>
-        <v>-18.214336990898609</v>
+        <v>-17.993189281413734</v>
       </c>
       <c r="L39" s="71">
         <f t="shared" si="10"/>
-        <v>-0.87114787388663395</v>
+        <v>-1.1102027783370756</v>
       </c>
       <c r="M39" s="72">
         <f t="shared" si="11"/>
-        <v>18.21447722598252</v>
+        <v>18.586796151085473</v>
       </c>
       <c r="N39" s="73">
         <f t="shared" si="12"/>
-        <v>-21.638558408519799</v>
+        <v>-20.763339828006092</v>
       </c>
       <c r="O39" s="65">
         <f t="shared" si="13"/>
-        <v>-8.5710439038768974E-2</v>
+        <v>-6.9309241291105578E-2</v>
       </c>
       <c r="P39" s="66">
         <f t="shared" si="14"/>
-        <v>34.871524561220696</v>
+        <v>34.93585756274426</v>
       </c>
       <c r="Q39" s="67">
         <f t="shared" si="15"/>
-        <v>-2.996059271557638</v>
+        <v>-1.8501647651614226</v>
       </c>
       <c r="R39" s="71">
         <f t="shared" si="16"/>
-        <v>0.69972699580909603</v>
+        <v>0.97158429575486438</v>
       </c>
       <c r="S39" s="72">
         <f t="shared" si="17"/>
-        <v>21.638698643603707</v>
+        <v>21.356946697677845</v>
       </c>
       <c r="T39" s="73">
         <f t="shared" si="18"/>
-        <v>18.214605928620411</v>
+        <v>19.140623207627524</v>
       </c>
     </row>
     <row r="40" spans="2:20" x14ac:dyDescent="0.25">
@@ -5241,75 +5040,75 @@
       </c>
       <c r="C40" s="65">
         <f t="shared" si="1"/>
-        <v>2.2990934658659978</v>
+        <v>2.4799067840586688</v>
       </c>
       <c r="D40" s="66">
         <f t="shared" si="2"/>
-        <v>-18.825172112470568</v>
+        <v>-19.046017363445763</v>
       </c>
       <c r="E40" s="67">
         <f t="shared" si="3"/>
-        <v>21.109632535089961</v>
+        <v>21.285096298689638</v>
       </c>
       <c r="F40" s="71">
         <f t="shared" si="4"/>
-        <v>3.0844523608972807</v>
+        <v>3.0953864927290562</v>
       </c>
       <c r="G40" s="72">
         <f t="shared" si="5"/>
-        <v>-34.942875252598988</v>
+        <v>-34.953802059436164</v>
       </c>
       <c r="H40" s="73">
         <f t="shared" si="6"/>
-        <v>1.998911839975027</v>
+        <v>1.9992884062000542</v>
       </c>
       <c r="I40" s="65">
         <f t="shared" si="7"/>
-        <v>-2.4133740512510227</v>
+        <v>-2.5723191057801427</v>
       </c>
       <c r="J40" s="66">
         <f t="shared" si="8"/>
-        <v>-21.109540264524604</v>
+        <v>-20.893606197523482</v>
       </c>
       <c r="K40" s="67">
         <f t="shared" si="9"/>
-        <v>-18.825084969180441</v>
+        <v>-18.67221111184783</v>
       </c>
       <c r="L40" s="71">
         <f t="shared" si="10"/>
-        <v>-0.84257772754037763</v>
+        <v>-1.0870996979067069</v>
       </c>
       <c r="M40" s="72">
         <f t="shared" si="11"/>
-        <v>18.825177239745798</v>
+        <v>19.063701213013974</v>
       </c>
       <c r="N40" s="73">
         <f t="shared" si="12"/>
-        <v>-21.10945312123448</v>
+        <v>-20.519799945925545</v>
       </c>
       <c r="O40" s="65">
         <f t="shared" si="13"/>
-        <v>-5.7140292692512626E-2</v>
+        <v>-4.6206160860737033E-2</v>
       </c>
       <c r="P40" s="66">
         <f t="shared" si="14"/>
-        <v>34.942880379874225</v>
+        <v>34.971485909004379</v>
       </c>
       <c r="Q40" s="67">
         <f t="shared" si="15"/>
-        <v>-1.9987324261195467</v>
+        <v>-1.2339920534359656</v>
       </c>
       <c r="R40" s="71">
         <f t="shared" si="16"/>
-        <v>0.72829714215535235</v>
+        <v>0.99468737618523295</v>
       </c>
       <c r="S40" s="72">
         <f t="shared" si="17"/>
-        <v>21.109545391799841</v>
+        <v>20.911290047091697</v>
       </c>
       <c r="T40" s="73">
         <f t="shared" si="18"/>
-        <v>18.825264383035922</v>
+        <v>19.437507464611908</v>
       </c>
     </row>
     <row r="41" spans="2:20" x14ac:dyDescent="0.25">
@@ -5318,75 +5117,75 @@
       </c>
       <c r="C41" s="65">
         <f t="shared" si="1"/>
-        <v>2.327663612212254</v>
+        <v>2.5030098644890373</v>
       </c>
       <c r="D41" s="66">
         <f t="shared" si="2"/>
-        <v>-19.420512186366274</v>
+        <v>-19.53043143267238</v>
       </c>
       <c r="E41" s="67">
         <f t="shared" si="3"/>
-        <v>20.563208089543348</v>
+        <v>20.648058378833856</v>
       </c>
       <c r="F41" s="71">
         <f t="shared" si="4"/>
-        <v>3.1130225072435369</v>
+        <v>3.1184895731594247</v>
       </c>
       <c r="G41" s="72">
         <f t="shared" si="5"/>
-        <v>-34.985715898486902</v>
+        <v>-34.988448973580795</v>
       </c>
       <c r="H41" s="73">
         <f t="shared" si="6"/>
-        <v>0.99986396334176308</v>
+        <v>0.99991104365317329</v>
       </c>
       <c r="I41" s="65">
         <f t="shared" si="7"/>
-        <v>-2.3848039049047665</v>
+        <v>-2.5492160253497742</v>
       </c>
       <c r="J41" s="66">
         <f t="shared" si="8"/>
-        <v>-20.563162576727148</v>
+        <v>-20.454472443261693</v>
       </c>
       <c r="K41" s="67">
         <f t="shared" si="9"/>
-        <v>-19.420467955630489</v>
+        <v>-19.341267049469508</v>
       </c>
       <c r="L41" s="71">
         <f t="shared" si="10"/>
-        <v>-0.81400758119412131</v>
+        <v>-1.0639966174763384</v>
       </c>
       <c r="M41" s="72">
         <f t="shared" si="11"/>
-        <v>19.420513468446686</v>
+        <v>19.53485298504166</v>
       </c>
       <c r="N41" s="73">
         <f t="shared" si="12"/>
-        <v>-20.563118345991366</v>
+        <v>-20.265308060058818</v>
       </c>
       <c r="O41" s="65">
         <f t="shared" si="13"/>
-        <v>-2.8570146346256313E-2</v>
+        <v>-2.3103080430368517E-2</v>
       </c>
       <c r="P41" s="66">
         <f t="shared" si="14"/>
-        <v>34.985717180567313</v>
+        <v>34.992870525950067</v>
       </c>
       <c r="Q41" s="67">
         <f t="shared" si="15"/>
-        <v>-0.99977421978977865</v>
+        <v>-0.61716072487813445</v>
       </c>
       <c r="R41" s="71">
         <f t="shared" si="16"/>
-        <v>0.75686728850160867</v>
+        <v>1.0177904566156015</v>
       </c>
       <c r="S41" s="72">
         <f t="shared" si="17"/>
-        <v>20.563163858807567</v>
+        <v>20.458893995630973</v>
       </c>
       <c r="T41" s="73">
         <f t="shared" si="18"/>
-        <v>19.420557699182467</v>
+        <v>19.724017368244535</v>
       </c>
     </row>
     <row r="42" spans="2:20" x14ac:dyDescent="0.25">
@@ -5395,7 +5194,7 @@
       </c>
       <c r="C42" s="79">
         <f t="shared" si="1"/>
-        <v>2.3562337585585102</v>
+        <v>2.5261129449194057</v>
       </c>
       <c r="D42" s="76">
         <f t="shared" si="2"/>
@@ -5403,7 +5202,7 @@
       </c>
       <c r="E42" s="77">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>20.000000000000004</v>
       </c>
       <c r="F42" s="79">
         <f t="shared" si="4"/>
@@ -5415,11 +5214,11 @@
       </c>
       <c r="H42" s="77">
         <f t="shared" si="6"/>
-        <v>4.2882120380498403E-15</v>
+        <v>5.3029658040673552E-15</v>
       </c>
       <c r="I42" s="79">
         <f t="shared" si="7"/>
-        <v>-2.3562337585585102</v>
+        <v>-2.5261129449194057</v>
       </c>
       <c r="J42" s="76">
         <f t="shared" si="8"/>
@@ -5427,11 +5226,11 @@
       </c>
       <c r="K42" s="77">
         <f t="shared" si="9"/>
-        <v>-20</v>
+        <v>-20.000000000000004</v>
       </c>
       <c r="L42" s="79">
         <f t="shared" si="10"/>
-        <v>-0.78543743484786499</v>
+        <v>-1.04089353704597</v>
       </c>
       <c r="M42" s="76">
         <f t="shared" si="11"/>
@@ -5455,7 +5254,7 @@
       </c>
       <c r="R42" s="79">
         <f t="shared" si="16"/>
-        <v>0.78543743484786499</v>
+        <v>1.04089353704597</v>
       </c>
       <c r="S42" s="76">
         <f t="shared" si="17"/>
@@ -5472,75 +5271,75 @@
       </c>
       <c r="C43" s="65">
         <f t="shared" si="1"/>
-        <v>2.3848039049047665</v>
+        <v>2.5492160253497742</v>
       </c>
       <c r="D43" s="66">
         <f t="shared" si="2"/>
-        <v>-20.563162576727148</v>
+        <v>-20.454472443261693</v>
       </c>
       <c r="E43" s="67">
         <f t="shared" si="3"/>
-        <v>19.420467955630489</v>
+        <v>19.341267049469508</v>
       </c>
       <c r="F43" s="71">
         <f t="shared" si="4"/>
-        <v>3.1701627999360493</v>
+        <v>3.1646957340201616</v>
       </c>
       <c r="G43" s="72">
         <f t="shared" si="5"/>
-        <v>-34.985715898486902</v>
+        <v>-34.988448973580795</v>
       </c>
       <c r="H43" s="73">
         <f t="shared" si="6"/>
-        <v>-0.99986396334175442</v>
+        <v>-0.99991104365316275</v>
       </c>
       <c r="I43" s="65">
         <f t="shared" si="7"/>
-        <v>-2.327663612212254</v>
+        <v>-2.5030098644890373</v>
       </c>
       <c r="J43" s="66">
         <f t="shared" si="8"/>
-        <v>-19.420512186366274</v>
+        <v>-19.53043143267238</v>
       </c>
       <c r="K43" s="67">
         <f t="shared" si="9"/>
-        <v>-20.563208089543348</v>
+        <v>-20.648058378833856</v>
       </c>
       <c r="L43" s="71">
         <f t="shared" si="10"/>
-        <v>-0.75686728850160867</v>
+        <v>-1.0177904566156015</v>
       </c>
       <c r="M43" s="72">
         <f t="shared" si="11"/>
-        <v>20.563163858807567</v>
+        <v>20.458893995630973</v>
       </c>
       <c r="N43" s="73">
         <f t="shared" si="12"/>
-        <v>-19.420557699182467</v>
+        <v>-19.724017368244535</v>
       </c>
       <c r="O43" s="65">
         <f t="shared" si="13"/>
-        <v>2.8570146346256344E-2</v>
+        <v>2.3103080430368544E-2</v>
       </c>
       <c r="P43" s="66">
         <f t="shared" si="14"/>
-        <v>34.985717180567313</v>
+        <v>34.992870525950067</v>
       </c>
       <c r="Q43" s="67">
         <f t="shared" si="15"/>
-        <v>0.99977421978977976</v>
+        <v>0.61716072487813523</v>
       </c>
       <c r="R43" s="71">
         <f t="shared" si="16"/>
-        <v>0.81400758119412131</v>
+        <v>1.0639966174763384</v>
       </c>
       <c r="S43" s="72">
         <f t="shared" si="17"/>
-        <v>19.420513468446686</v>
+        <v>19.53485298504166</v>
       </c>
       <c r="T43" s="73">
         <f t="shared" si="18"/>
-        <v>20.563118345991366</v>
+        <v>20.265308060058818</v>
       </c>
     </row>
     <row r="44" spans="2:20" x14ac:dyDescent="0.25">
@@ -5549,75 +5348,75 @@
       </c>
       <c r="C44" s="65">
         <f t="shared" si="1"/>
-        <v>2.4133740512510227</v>
+        <v>2.5723191057801427</v>
       </c>
       <c r="D44" s="66">
         <f t="shared" si="2"/>
-        <v>-21.109540264524604</v>
+        <v>-20.893606197523482</v>
       </c>
       <c r="E44" s="67">
         <f t="shared" si="3"/>
-        <v>18.825084969180441</v>
+        <v>18.67221111184783</v>
       </c>
       <c r="F44" s="71">
         <f t="shared" si="4"/>
-        <v>3.1987329462823055</v>
+        <v>3.18779881445053</v>
       </c>
       <c r="G44" s="72">
         <f t="shared" si="5"/>
-        <v>-34.942875252598988</v>
+        <v>-34.953802059436164</v>
       </c>
       <c r="H44" s="73">
         <f t="shared" si="6"/>
-        <v>-1.9989118399750183</v>
+        <v>-1.9992884062000433</v>
       </c>
       <c r="I44" s="65">
         <f t="shared" si="7"/>
-        <v>-2.2990934658659978</v>
+        <v>-2.4799067840586688</v>
       </c>
       <c r="J44" s="66">
         <f t="shared" si="8"/>
-        <v>-18.825172112470568</v>
+        <v>-19.046017363445763</v>
       </c>
       <c r="K44" s="67">
         <f t="shared" si="9"/>
-        <v>-21.109632535089961</v>
+        <v>-21.285096298689638</v>
       </c>
       <c r="L44" s="71">
         <f t="shared" si="10"/>
-        <v>-0.72829714215535235</v>
+        <v>-0.99468737618523295</v>
       </c>
       <c r="M44" s="72">
         <f t="shared" si="11"/>
-        <v>21.109545391799841</v>
+        <v>20.911290047091697</v>
       </c>
       <c r="N44" s="73">
         <f t="shared" si="12"/>
-        <v>-18.825264383035922</v>
+        <v>-19.437507464611908</v>
       </c>
       <c r="O44" s="65">
         <f t="shared" si="13"/>
-        <v>5.7140292692512626E-2</v>
+        <v>4.6206160860737033E-2</v>
       </c>
       <c r="P44" s="66">
         <f t="shared" si="14"/>
-        <v>34.942880379874225</v>
+        <v>34.971485909004379</v>
       </c>
       <c r="Q44" s="67">
         <f t="shared" si="15"/>
-        <v>1.9987324261195467</v>
+        <v>1.2339920534359656</v>
       </c>
       <c r="R44" s="71">
         <f t="shared" si="16"/>
-        <v>0.84257772754037763</v>
+        <v>1.0870996979067069</v>
       </c>
       <c r="S44" s="72">
         <f t="shared" si="17"/>
-        <v>18.825177239745798</v>
+        <v>19.063701213013974</v>
       </c>
       <c r="T44" s="73">
         <f t="shared" si="18"/>
-        <v>21.10945312123448</v>
+        <v>20.519799945925545</v>
       </c>
     </row>
     <row r="45" spans="2:20" x14ac:dyDescent="0.25">
@@ -5626,75 +5425,75 @@
       </c>
       <c r="C45" s="65">
         <f t="shared" si="1"/>
-        <v>2.4419441975972793</v>
+        <v>2.5954221862105111</v>
       </c>
       <c r="D45" s="66">
         <f t="shared" si="2"/>
-        <v>-21.63868711115769</v>
+        <v>-21.317166884548143</v>
       </c>
       <c r="E45" s="67">
         <f t="shared" si="3"/>
-        <v>18.214336990898609</v>
+        <v>17.993189281413734</v>
       </c>
       <c r="F45" s="71">
         <f t="shared" si="4"/>
-        <v>3.2273030926285622</v>
+        <v>3.2109018948808985</v>
       </c>
       <c r="G45" s="72">
         <f t="shared" si="5"/>
-        <v>-34.871513028774679</v>
+        <v>-34.896077749614562</v>
       </c>
       <c r="H45" s="73">
         <f t="shared" si="6"/>
-        <v>-2.9963282092794357</v>
+        <v>-2.9975986913752113</v>
       </c>
       <c r="I45" s="65">
         <f t="shared" si="7"/>
-        <v>-2.2705233195197412</v>
+        <v>-2.4568037036283004</v>
       </c>
       <c r="J45" s="66">
         <f t="shared" si="8"/>
-        <v>-18.2144656935365</v>
+        <v>-18.547016337955782</v>
       </c>
       <c r="K45" s="67">
         <f t="shared" si="9"/>
-        <v>-21.638827346241598</v>
+        <v>-21.910773754219893</v>
       </c>
       <c r="L45" s="71">
         <f t="shared" si="10"/>
-        <v>-0.69972699580909603</v>
+        <v>-0.97158429575486438</v>
       </c>
       <c r="M45" s="72">
         <f t="shared" si="11"/>
-        <v>21.638698643603707</v>
+        <v>21.356946697677845</v>
       </c>
       <c r="N45" s="73">
         <f t="shared" si="12"/>
-        <v>-18.214605928620411</v>
+        <v>-19.140623207627524</v>
       </c>
       <c r="O45" s="65">
         <f t="shared" si="13"/>
-        <v>8.5710439038768974E-2</v>
+        <v>6.9309241291105578E-2</v>
       </c>
       <c r="P45" s="66">
         <f t="shared" si="14"/>
-        <v>34.871524561220696</v>
+        <v>34.93585756274426</v>
       </c>
       <c r="Q45" s="67">
         <f t="shared" si="15"/>
-        <v>2.996059271557638</v>
+        <v>1.8501647651614226</v>
       </c>
       <c r="R45" s="71">
         <f t="shared" si="16"/>
-        <v>0.87114787388663395</v>
+        <v>1.1102027783370756</v>
       </c>
       <c r="S45" s="72">
         <f t="shared" si="17"/>
-        <v>18.21447722598252</v>
+        <v>18.586796151085473</v>
       </c>
       <c r="T45" s="73">
         <f t="shared" si="18"/>
-        <v>21.638558408519799</v>
+        <v>20.763339828006092</v>
       </c>
     </row>
     <row r="46" spans="2:20" x14ac:dyDescent="0.25">
@@ -5703,75 +5502,75 @@
       </c>
       <c r="C46" s="65">
         <f t="shared" si="1"/>
-        <v>2.4705143439435355</v>
+        <v>2.61852526664088</v>
       </c>
       <c r="D46" s="66">
         <f t="shared" si="2"/>
-        <v>-22.150171228165355</v>
+        <v>-21.724928437889609</v>
       </c>
       <c r="E46" s="67">
         <f t="shared" si="3"/>
-        <v>17.588722511905392</v>
+        <v>17.304563971527834</v>
       </c>
       <c r="F46" s="71">
         <f t="shared" si="4"/>
-        <v>3.2558732389748184</v>
+        <v>3.234004975311267</v>
       </c>
       <c r="G46" s="72">
         <f t="shared" si="5"/>
-        <v>-34.771687472699867</v>
+        <v>-34.81530685323019</v>
       </c>
       <c r="H46" s="73">
         <f t="shared" si="6"/>
-        <v>-3.9912989822672063</v>
+        <v>-3.994309072442936</v>
       </c>
       <c r="I46" s="65">
         <f t="shared" si="7"/>
-        <v>-2.241953173173485</v>
+        <v>-2.4337006231979315</v>
       </c>
       <c r="J46" s="66">
         <f t="shared" si="8"/>
-        <v>-17.58889138676383</v>
+        <v>-18.033694687313591</v>
       </c>
       <c r="K46" s="67">
         <f t="shared" si="9"/>
-        <v>-22.150360595388669</v>
+        <v>-22.524756803481743</v>
       </c>
       <c r="L46" s="71">
         <f t="shared" si="10"/>
-        <v>-0.67115684946283971</v>
+        <v>-0.94848121532449592</v>
       </c>
       <c r="M46" s="72">
         <f t="shared" si="11"/>
-        <v>22.150191720530227</v>
+        <v>21.795626087695972</v>
       </c>
       <c r="N46" s="73">
         <f t="shared" si="12"/>
-        <v>-17.589080753987144</v>
+        <v>-18.833523052905722</v>
       </c>
       <c r="O46" s="65">
         <f t="shared" si="13"/>
-        <v>0.11428058538502525</v>
+        <v>9.2412321721474067E-2</v>
       </c>
       <c r="P46" s="66">
         <f t="shared" si="14"/>
-        <v>34.771707965064742</v>
+        <v>34.886004503036553</v>
       </c>
       <c r="Q46" s="67">
         <f t="shared" si="15"/>
-        <v>3.9909407401854557</v>
+        <v>2.4653499910650618</v>
       </c>
       <c r="R46" s="71">
         <f t="shared" si="16"/>
-        <v>0.89971802023289027</v>
+        <v>1.1333058587674441</v>
       </c>
       <c r="S46" s="72">
         <f t="shared" si="17"/>
-        <v>17.588911879128705</v>
+        <v>18.104392337119965</v>
       </c>
       <c r="T46" s="73">
         <f t="shared" si="18"/>
-        <v>22.150002353306913</v>
+        <v>20.995797722103841</v>
       </c>
     </row>
     <row r="47" spans="2:20" x14ac:dyDescent="0.25">
@@ -5780,75 +5579,75 @@
       </c>
       <c r="C47" s="65">
         <f t="shared" si="1"/>
-        <v>2.4990844902897917</v>
+        <v>2.6416283470712485</v>
       </c>
       <c r="D47" s="66">
         <f t="shared" si="2"/>
-        <v>-22.643575143366586</v>
+        <v>-22.116673223551054</v>
       </c>
       <c r="E47" s="67">
         <f t="shared" si="3"/>
-        <v>16.948752157325458</v>
+        <v>16.606702721202282</v>
       </c>
       <c r="F47" s="71">
         <f t="shared" si="4"/>
-        <v>3.2844433853210746</v>
+        <v>3.2571080557416359</v>
       </c>
       <c r="G47" s="72">
         <f t="shared" si="5"/>
-        <v>-34.643480061767946</v>
+        <v>-34.711532480019251</v>
       </c>
       <c r="H47" s="73">
         <f t="shared" si="6"/>
-        <v>-4.9830120660407644</v>
+        <v>-4.9888875765820613</v>
       </c>
       <c r="I47" s="65">
         <f t="shared" si="7"/>
-        <v>-2.2133830268272288</v>
+        <v>-2.410597542767563</v>
       </c>
       <c r="J47" s="66">
         <f t="shared" si="8"/>
-        <v>-16.94895978448875</v>
+        <v>-17.506326385957379</v>
       </c>
       <c r="K47" s="67">
         <f t="shared" si="9"/>
-        <v>-22.643814770248621</v>
+        <v>-23.126717746171163</v>
       </c>
       <c r="L47" s="71">
         <f t="shared" si="10"/>
-        <v>-0.64258670311658339</v>
+        <v>-0.92537813489412735</v>
       </c>
       <c r="M47" s="72">
         <f t="shared" si="11"/>
-        <v>22.64360714308533</v>
+        <v>22.227094081416055</v>
       </c>
       <c r="N47" s="73">
         <f t="shared" si="12"/>
-        <v>-16.949199411370785</v>
+        <v>-18.516370908577485</v>
       </c>
       <c r="O47" s="65">
         <f t="shared" si="13"/>
-        <v>0.1428507317312816</v>
+        <v>0.11551540215184261</v>
       </c>
       <c r="P47" s="66">
         <f t="shared" si="14"/>
-        <v>34.643512061486689</v>
+        <v>34.821953337884253</v>
       </c>
       <c r="Q47" s="67">
         <f t="shared" si="15"/>
-        <v>4.9825648119954424</v>
+        <v>3.0792193892068549</v>
       </c>
       <c r="R47" s="71">
         <f t="shared" si="16"/>
-        <v>0.92828816657914659</v>
+        <v>1.1564089391978125</v>
       </c>
       <c r="S47" s="72">
         <f t="shared" si="17"/>
-        <v>16.948991784207493</v>
+        <v>17.616747243822388</v>
       </c>
       <c r="T47" s="73">
         <f t="shared" si="18"/>
-        <v>22.643367516203291</v>
+        <v>21.217049558795946</v>
       </c>
     </row>
     <row r="48" spans="2:20" x14ac:dyDescent="0.25">
@@ -5857,75 +5656,75 @@
       </c>
       <c r="C48" s="65">
         <f t="shared" si="1"/>
-        <v>2.5276546366360484</v>
+        <v>2.664731427501617</v>
       </c>
       <c r="D48" s="66">
         <f t="shared" si="2"/>
-        <v>-23.118496141600247</v>
+        <v>-22.492192156142416</v>
       </c>
       <c r="E48" s="67">
         <f t="shared" si="3"/>
-        <v>16.294948269516713</v>
+        <v>15.899977998934611</v>
       </c>
       <c r="F48" s="71">
         <f t="shared" si="4"/>
-        <v>3.3130135316673313</v>
+        <v>3.2802111361720043</v>
       </c>
       <c r="G48" s="72">
         <f t="shared" si="5"/>
-        <v>-34.486995438578141</v>
+        <v>-34.584810017331122</v>
       </c>
       <c r="H48" s="73">
         <f t="shared" si="6"/>
-        <v>-5.9706580266211242</v>
+        <v>-5.9808033688150299</v>
       </c>
       <c r="I48" s="65">
         <f t="shared" si="7"/>
-        <v>-2.1848128804809721</v>
+        <v>-2.3874944623371945</v>
       </c>
       <c r="J48" s="66">
         <f t="shared" si="8"/>
-        <v>-16.29519319743962</v>
+        <v>-16.965192905424296</v>
       </c>
       <c r="K48" s="67">
         <f t="shared" si="9"/>
-        <v>-23.118787114638501</v>
+        <v>-23.716335298526101</v>
       </c>
       <c r="L48" s="71">
         <f t="shared" si="10"/>
-        <v>-0.61401655677032707</v>
+        <v>-0.90227505446375877</v>
       </c>
       <c r="M48" s="72">
         <f t="shared" si="11"/>
-        <v>23.118542186715594</v>
+        <v>22.651120392036404</v>
       </c>
       <c r="N48" s="73">
         <f t="shared" si="12"/>
-        <v>-16.295484170477884</v>
+        <v>-18.189336047807981</v>
       </c>
       <c r="O48" s="65">
         <f t="shared" si="13"/>
-        <v>0.17142087807753795</v>
+        <v>0.13861848258221116</v>
       </c>
       <c r="P48" s="66">
         <f t="shared" si="14"/>
-        <v>34.487041483693488</v>
+        <v>34.743738253225104</v>
       </c>
       <c r="Q48" s="67">
         <f t="shared" si="15"/>
-        <v>5.9701221256599561</v>
+        <v>3.6914453199416584</v>
       </c>
       <c r="R48" s="71">
         <f t="shared" si="16"/>
-        <v>0.95685831292540291</v>
+        <v>1.1795120196281812</v>
       </c>
       <c r="S48" s="72">
         <f t="shared" si="17"/>
-        <v>16.295239242554977</v>
+        <v>17.124121141318291</v>
       </c>
       <c r="T48" s="73">
         <f t="shared" si="18"/>
-        <v>23.118251213677333</v>
+        <v>21.426977249652715</v>
       </c>
     </row>
     <row r="49" spans="2:20" x14ac:dyDescent="0.25">
@@ -5934,75 +5733,75 @@
       </c>
       <c r="C49" s="65">
         <f t="shared" si="1"/>
-        <v>2.5562247829823046</v>
+        <v>2.6878345079319854</v>
       </c>
       <c r="D49" s="66">
         <f t="shared" si="2"/>
-        <v>-23.574546593420266</v>
+        <v>-22.851284810475221</v>
       </c>
       <c r="E49" s="67">
         <f t="shared" si="3"/>
-        <v>15.627844481735664</v>
+        <v>15.184767003910704</v>
       </c>
       <c r="F49" s="71">
         <f t="shared" si="4"/>
-        <v>3.3415836780135875</v>
+        <v>3.3033142166023728</v>
       </c>
       <c r="G49" s="72">
         <f t="shared" si="5"/>
-        <v>-34.302361325526448</v>
+        <v>-34.435207100566458</v>
       </c>
       <c r="H49" s="73">
         <f t="shared" si="6"/>
-        <v>-6.9534307496060181</v>
+        <v>-6.9695270353298016</v>
       </c>
       <c r="I49" s="65">
         <f t="shared" si="7"/>
-        <v>-2.1562427341347159</v>
+        <v>-2.3643913819068261</v>
       </c>
       <c r="J49" s="66">
         <f t="shared" si="8"/>
-        <v>-15.628125228428157</v>
+        <v>-16.410583064121127</v>
       </c>
       <c r="K49" s="67">
         <f t="shared" si="9"/>
-        <v>-23.574889957203627</v>
+        <v>-24.293294764804742</v>
       </c>
       <c r="L49" s="71">
         <f t="shared" si="10"/>
-        <v>-0.58544641042407075</v>
+        <v>-0.87917197403339031</v>
       </c>
       <c r="M49" s="72">
         <f t="shared" si="11"/>
-        <v>23.574609210511134</v>
+        <v>23.067478704594315</v>
       </c>
       <c r="N49" s="73">
         <f t="shared" si="12"/>
-        <v>-15.628468592211515</v>
+        <v>-17.852593018450641</v>
       </c>
       <c r="O49" s="65">
         <f t="shared" si="13"/>
-        <v>0.19999102442379424</v>
+        <v>0.16172156301257964</v>
       </c>
       <c r="P49" s="66">
         <f t="shared" si="14"/>
-        <v>34.302423942617317</v>
+        <v>34.651400994685552</v>
       </c>
       <c r="Q49" s="67">
         <f t="shared" si="15"/>
-        <v>6.9528066391301708</v>
+        <v>4.3017010207898609</v>
       </c>
       <c r="R49" s="71">
         <f t="shared" si="16"/>
-        <v>0.98542845927165923</v>
+        <v>1.2026151000585497</v>
       </c>
       <c r="S49" s="72">
         <f t="shared" si="17"/>
-        <v>15.628187845519026</v>
+        <v>16.626776958240217</v>
       </c>
       <c r="T49" s="73">
         <f t="shared" si="18"/>
-        <v>23.574265846727776</v>
+        <v>21.625468750264794</v>
       </c>
     </row>
     <row r="50" spans="2:20" x14ac:dyDescent="0.25">
@@ -6011,75 +5810,75 @@
       </c>
       <c r="C50" s="65">
         <f t="shared" si="1"/>
-        <v>2.5847949293285608</v>
+        <v>2.7109375883623539</v>
       </c>
       <c r="D50" s="66">
         <f t="shared" si="2"/>
-        <v>-24.011354271477963</v>
+        <v>-23.19375952853526</v>
       </c>
       <c r="E50" s="67">
         <f t="shared" si="3"/>
-        <v>14.94798528258711</v>
+        <v>14.461451464682787</v>
       </c>
       <c r="F50" s="71">
         <f t="shared" si="4"/>
-        <v>3.3701538243598437</v>
+        <v>3.3264172970327412</v>
       </c>
       <c r="G50" s="72">
         <f t="shared" si="5"/>
-        <v>-34.089728420558906</v>
+        <v>-34.26280357707833</v>
       </c>
       <c r="H50" s="73">
         <f t="shared" si="6"/>
-        <v>-7.9305280981187396</v>
+        <v>-7.9545308660430551</v>
       </c>
       <c r="I50" s="65">
         <f t="shared" si="7"/>
-        <v>-2.1276725877884597</v>
+        <v>-2.3412883014764576</v>
       </c>
       <c r="J50" s="66">
         <f t="shared" si="8"/>
-        <v>-14.94830033682395</v>
+        <v>-15.842792873173584</v>
       </c>
       <c r="K50" s="67">
         <f t="shared" si="9"/>
-        <v>-24.011751027834091</v>
+        <v>-24.857288205247652</v>
       </c>
       <c r="L50" s="71">
         <f t="shared" si="10"/>
-        <v>-0.55687626407781443</v>
+        <v>-0.85606889360302185</v>
       </c>
       <c r="M50" s="72">
         <f t="shared" si="11"/>
-        <v>24.011435973597251</v>
+        <v>23.475946796756844</v>
       </c>
       <c r="N50" s="73">
         <f t="shared" si="12"/>
-        <v>-14.948697093180078</v>
+        <v>-17.506321549885975</v>
       </c>
       <c r="O50" s="65">
         <f t="shared" si="13"/>
-        <v>0.22856117077005056</v>
+        <v>0.18482464344294819</v>
       </c>
       <c r="P50" s="66">
         <f t="shared" si="14"/>
-        <v>34.089810122678202</v>
+        <v>34.544990845299921</v>
       </c>
       <c r="Q50" s="67">
         <f t="shared" si="15"/>
-        <v>7.9298162875257772</v>
+        <v>4.909660780839868</v>
       </c>
       <c r="R50" s="71">
         <f t="shared" si="16"/>
-        <v>1.0139986056179155</v>
+        <v>1.2257181804889181</v>
       </c>
       <c r="S50" s="72">
         <f t="shared" si="17"/>
-        <v>14.948382038943242</v>
+        <v>16.124980141395174</v>
       </c>
       <c r="T50" s="73">
         <f t="shared" si="18"/>
-        <v>24.011039217241123</v>
+        <v>21.812418120044455</v>
       </c>
     </row>
     <row r="51" spans="2:20" x14ac:dyDescent="0.25">
@@ -6088,75 +5887,75 @@
       </c>
       <c r="C51" s="65">
         <f t="shared" si="1"/>
-        <v>2.613365075674817</v>
+        <v>2.7340406687927223</v>
       </c>
       <c r="D51" s="66">
         <f t="shared" si="2"/>
-        <v>-24.42856265433311</v>
+        <v>-23.519433521775909</v>
       </c>
       <c r="E51" s="67">
         <f t="shared" si="3"/>
-        <v>14.255925571613801</v>
+        <v>13.730417435430004</v>
       </c>
       <c r="F51" s="71">
         <f t="shared" si="4"/>
-        <v>3.3987239707060999</v>
+        <v>3.3495203774631097</v>
       </c>
       <c r="G51" s="72">
         <f t="shared" si="5"/>
-        <v>-33.849270274172284</v>
+        <v>-34.067691463555342</v>
       </c>
       <c r="H51" s="73">
         <f t="shared" si="6"/>
-        <v>-8.9011525675103975</v>
+        <v>-8.9352891362541698</v>
       </c>
       <c r="I51" s="65">
         <f t="shared" si="7"/>
-        <v>-2.0991024414422035</v>
+        <v>-2.3181852210460892</v>
       </c>
       <c r="J51" s="66">
         <f t="shared" si="8"/>
-        <v>-14.256273394168016</v>
+        <v>-15.262125378436776</v>
       </c>
       <c r="K51" s="67">
         <f t="shared" si="9"/>
-        <v>-24.429013761510788</v>
+        <v>-25.408014600434004</v>
       </c>
       <c r="L51" s="71">
         <f t="shared" si="10"/>
-        <v>-0.52830611773155811</v>
+        <v>-0.83296581317265328</v>
       </c>
       <c r="M51" s="72">
         <f t="shared" si="11"/>
-        <v>24.428665938956573</v>
+        <v>23.876306657427222</v>
       </c>
       <c r="N51" s="73">
         <f t="shared" si="12"/>
-        <v>-14.256724501345689</v>
+        <v>-17.150706457094863</v>
       </c>
       <c r="O51" s="65">
         <f t="shared" si="13"/>
-        <v>0.25713131711630688</v>
+        <v>0.20792772387331668</v>
       </c>
       <c r="P51" s="66">
         <f t="shared" si="14"/>
-        <v>33.849373558795747</v>
+        <v>34.424564599206647</v>
       </c>
       <c r="Q51" s="67">
         <f t="shared" si="15"/>
-        <v>8.9003536377785153</v>
+        <v>5.5150001145893075</v>
       </c>
       <c r="R51" s="71">
         <f t="shared" si="16"/>
-        <v>1.042568751964172</v>
+        <v>1.2488212609192866</v>
       </c>
       <c r="S51" s="72">
         <f t="shared" si="17"/>
-        <v>14.256376678791474</v>
+        <v>15.618998514088089</v>
       </c>
       <c r="T51" s="73">
         <f t="shared" si="18"/>
-        <v>24.428214831778899</v>
+        <v>21.98772557876913</v>
       </c>
     </row>
     <row r="52" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6165,79 +5964,111 @@
       </c>
       <c r="C52" s="88">
         <f t="shared" si="1"/>
-        <v>2.6419352220210737</v>
+        <v>2.7571437492230908</v>
       </c>
       <c r="D52" s="89">
         <f t="shared" si="2"/>
-        <v>-24.825831217445973</v>
+        <v>-23.82813296867765</v>
       </c>
       <c r="E52" s="90">
         <f t="shared" si="3"/>
-        <v>13.552230206388673</v>
+        <v>12.992055089910252</v>
       </c>
       <c r="F52" s="91">
         <f t="shared" si="4"/>
-        <v>3.4272941170523561</v>
+        <v>3.3726234578934782</v>
       </c>
       <c r="G52" s="92">
         <f t="shared" si="5"/>
-        <v>-33.581183147762538</v>
+        <v>-33.849974896909735</v>
       </c>
       <c r="H52" s="93">
         <f t="shared" si="6"/>
-        <v>-9.8645119362814118</v>
+        <v>-9.9112783872395216</v>
       </c>
       <c r="I52" s="88">
         <f t="shared" si="7"/>
-        <v>-2.0705322950959468</v>
+        <v>-2.2950821406157207</v>
       </c>
       <c r="J52" s="89">
         <f t="shared" si="8"/>
-        <v>-13.552609231287864</v>
+        <v>-14.668890498750928</v>
       </c>
       <c r="K52" s="90">
         <f t="shared" si="9"/>
-        <v>-24.826337589332955</v>
+        <v>-25.945180011944267</v>
       </c>
       <c r="L52" s="91">
         <f t="shared" si="10"/>
-        <v>-0.49973597138530179</v>
+        <v>-0.80986273274228471</v>
       </c>
       <c r="M52" s="92">
         <f t="shared" si="11"/>
-        <v>24.825958564433762</v>
+        <v>24.268344603103579</v>
       </c>
       <c r="N52" s="93">
         <f t="shared" si="12"/>
-        <v>-13.553115603174851</v>
+        <v>-16.785937542017532</v>
       </c>
       <c r="O52" s="88">
         <f t="shared" si="13"/>
-        <v>0.2857014634625632</v>
+        <v>0.23103080430368522</v>
       </c>
       <c r="P52" s="89">
         <f t="shared" si="14"/>
-        <v>33.581310494750326</v>
+        <v>34.29018653133565</v>
       </c>
       <c r="Q52" s="90">
         <f t="shared" si="15"/>
-        <v>9.8636265394952538</v>
+        <v>6.1173959351322393</v>
       </c>
       <c r="R52" s="91">
         <f t="shared" si="16"/>
-        <v>1.0711388983104282</v>
+        <v>1.2719243413496553</v>
       </c>
       <c r="S52" s="92">
         <f t="shared" si="17"/>
-        <v>13.552736578275663</v>
+        <v>15.109102133176851</v>
       </c>
       <c r="T52" s="93">
         <f t="shared" si="18"/>
-        <v>24.825452192546781</v>
+        <v>22.151297559836966</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B5:M5"/>
+    <mergeCell ref="B11:M11"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="G26:M26"/>
+    <mergeCell ref="G13:M18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="G19:M24"/>
     <mergeCell ref="B29:T29"/>
@@ -6254,38 +6085,6 @@
     <mergeCell ref="R30:T30"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:M25"/>
-    <mergeCell ref="G12:M12"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="G26:M26"/>
-    <mergeCell ref="G13:M18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B5:M5"/>
-    <mergeCell ref="B11:M11"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6301,7 +6100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6312,7 +6111,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B2" s="52">
         <v>25</v>

</xml_diff>